<commit_message>
added union results. exceptional
</commit_message>
<xml_diff>
--- a/misc/union_results.xlsx
+++ b/misc/union_results.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5BBF0D-1755-984C-A2EA-E9342881CB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4CAF1E5-8E9B-7E4E-AAEC-2BE5D88E11C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="6860" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="6860" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
-    <sheet name="llm" sheetId="11" r:id="rId2"/>
-    <sheet name="llm-correction" sheetId="9" r:id="rId3"/>
+    <sheet name="llm (all)" sheetId="11" r:id="rId2"/>
+    <sheet name="llm (main)" sheetId="12" r:id="rId3"/>
+    <sheet name="llm (ablation)" sheetId="13" r:id="rId4"/>
+    <sheet name="llm-correction" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="36">
   <si>
     <t>4o-mini</t>
   </si>
@@ -88,22 +90,7 @@
     <t>qwen</t>
   </si>
   <si>
-    <t>zs-comb</t>
-  </si>
-  <si>
-    <t>fs-comb</t>
-  </si>
-  <si>
-    <t>models</t>
-  </si>
-  <si>
-    <t>min_angle thresholds</t>
-  </si>
-  <si>
     <t>llm results</t>
-  </si>
-  <si>
-    <t>external correction results</t>
   </si>
   <si>
     <t>worst</t>
@@ -113,18 +100,6 @@
   </si>
   <si>
     <t>avg</t>
-  </si>
-  <si>
-    <t>zs</t>
-  </si>
-  <si>
-    <t>fs</t>
-  </si>
-  <si>
-    <t>zs-all</t>
-  </si>
-  <si>
-    <t>fs-all</t>
   </si>
   <si>
     <t>area</t>
@@ -167,6 +142,12 @@
   </si>
   <si>
     <t>best (a=5, m=0.5)</t>
+  </si>
+  <si>
+    <t>ZeroShot</t>
+  </si>
+  <si>
+    <t>FewShot</t>
   </si>
 </sst>
 </file>
@@ -407,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -439,19 +420,10 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -469,12 +441,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -500,9 +466,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -520,18 +483,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -598,6 +549,60 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -607,65 +612,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1005,7 +956,7 @@
   <dimension ref="B2:R35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1027,87 +978,87 @@
   <sheetData>
     <row r="2" spans="2:18" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="59" t="s">
+      <c r="C3" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="61"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="23" t="s">
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="51"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="R3" s="24" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="4" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="18">
         <v>1</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="35">
         <v>0.85699999999999998</v>
       </c>
-      <c r="F4" s="59"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60" t="s">
+      <c r="F4" s="49"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="61"/>
-      <c r="N4" s="30" t="s">
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="51"/>
+      <c r="N4" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="O4" s="26">
+      <c r="O4" s="21">
         <f>MIN($D$4:$D$8)</f>
         <v>0.84199999999999997</v>
       </c>
-      <c r="P4" s="26">
+      <c r="P4" s="21">
         <f>MAX($D$4:$D$8)</f>
         <v>0.86699999999999999</v>
       </c>
-      <c r="Q4" s="26">
+      <c r="Q4" s="21">
         <f>AVERAGE($D$4:$D$8)</f>
         <v>0.85299999999999998</v>
       </c>
-      <c r="R4" s="27">
+      <c r="R4" s="22">
         <f>STDEV($D$4:$D$8)</f>
         <v>1.0839741694339409E-2</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="57"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="22">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F5" s="62"/>
-      <c r="G5" s="63"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="1">
         <v>0.5</v>
       </c>
@@ -1120,411 +1071,411 @@
       <c r="K5" s="1">
         <v>0.8</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="20">
         <v>0.9</v>
       </c>
-      <c r="M5" s="26"/>
-      <c r="N5" s="30" t="s">
+      <c r="M5" s="21"/>
+      <c r="N5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="26">
+      <c r="O5" s="21">
         <f>MIN($D$9:$D$13)</f>
         <v>0.88200000000000001</v>
       </c>
-      <c r="P5" s="26">
+      <c r="P5" s="21">
         <f>MAX($D$9:$D$13)</f>
         <v>0.92700000000000005</v>
       </c>
-      <c r="Q5" s="26">
+      <c r="Q5" s="21">
         <f>AVERAGE($D$9:$D$13)</f>
         <v>0.90760000000000007</v>
       </c>
-      <c r="R5" s="27">
+      <c r="R5" s="22">
         <f>STDEV($D$9:$D$13)</f>
         <v>1.7008821240756238E-2</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="57"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="22">
         <v>0.85699999999999998</v>
       </c>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="47" t="s">
         <v>4</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="52">
+      <c r="H6" s="42">
         <v>0.92230599999999996</v>
       </c>
-      <c r="I6" s="52">
+      <c r="I6" s="42">
         <v>0.90977399999999997</v>
       </c>
-      <c r="J6" s="52">
+      <c r="J6" s="42">
         <v>0.90476199999999996</v>
       </c>
-      <c r="K6" s="52">
+      <c r="K6" s="42">
         <v>0.90225599999999995</v>
       </c>
-      <c r="L6" s="42">
+      <c r="L6" s="32">
         <v>0.86967399999999995</v>
       </c>
-      <c r="M6" s="26"/>
-      <c r="N6" s="31" t="s">
+      <c r="M6" s="21"/>
+      <c r="N6" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="O6" s="28">
+      <c r="O6" s="23">
         <f>MIN($H$6:$L$10)</f>
         <v>0.86967399999999995</v>
       </c>
-      <c r="P6" s="28">
+      <c r="P6" s="23">
         <f>MAX($H$6:$L$10)</f>
         <v>0.96240599999999998</v>
       </c>
-      <c r="Q6" s="28">
+      <c r="Q6" s="23">
         <f>AVERAGE($H$6:$L$10)</f>
         <v>0.93323307999999994</v>
       </c>
-      <c r="R6" s="29">
+      <c r="R6" s="24">
         <f>STDEV($H$6:$L$10)</f>
         <v>2.3341873105572904E-2</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="57"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="1">
         <v>4</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="22">
         <v>0.84199999999999997</v>
       </c>
-      <c r="F7" s="57"/>
+      <c r="F7" s="47"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
-      <c r="H7" s="52">
+      <c r="H7" s="42">
         <v>0.95488700000000004</v>
       </c>
-      <c r="I7" s="52">
+      <c r="I7" s="42">
         <v>0.94486199999999998</v>
       </c>
-      <c r="J7" s="52">
+      <c r="J7" s="42">
         <v>0.93984999999999996</v>
       </c>
-      <c r="K7" s="52">
+      <c r="K7" s="42">
         <v>0.93734300000000004</v>
       </c>
-      <c r="L7" s="42">
+      <c r="L7" s="32">
         <v>0.90225599999999995</v>
       </c>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="26"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
     </row>
     <row r="8" spans="2:18" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="58"/>
-      <c r="C8" s="16">
+      <c r="B8" s="48"/>
+      <c r="C8" s="13">
         <v>5</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="24">
         <v>0.84199999999999997</v>
       </c>
-      <c r="F8" s="57"/>
+      <c r="F8" s="47"/>
       <c r="G8" s="1">
         <v>5</v>
       </c>
-      <c r="H8" s="52">
+      <c r="H8" s="42">
         <v>0.96240599999999998</v>
       </c>
-      <c r="I8" s="52">
+      <c r="I8" s="42">
         <v>0.95238100000000003</v>
       </c>
-      <c r="J8" s="52">
+      <c r="J8" s="42">
         <v>0.94987500000000002</v>
       </c>
-      <c r="K8" s="52">
+      <c r="K8" s="42">
         <v>0.94486199999999998</v>
       </c>
-      <c r="L8" s="42">
+      <c r="L8" s="32">
         <v>0.91228100000000001</v>
       </c>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
     </row>
     <row r="9" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="18">
         <v>0.5</v>
       </c>
-      <c r="D9" s="45">
+      <c r="D9" s="35">
         <v>0.88200000000000001</v>
       </c>
-      <c r="F9" s="57"/>
+      <c r="F9" s="47"/>
       <c r="G9" s="1">
         <v>10</v>
       </c>
-      <c r="H9" s="52">
+      <c r="H9" s="42">
         <v>0.95238100000000003</v>
       </c>
-      <c r="I9" s="52">
+      <c r="I9" s="42">
         <v>0.94736799999999999</v>
       </c>
-      <c r="J9" s="52">
+      <c r="J9" s="42">
         <v>0.94736799999999999</v>
       </c>
-      <c r="K9" s="52">
+      <c r="K9" s="42">
         <v>0.94486199999999998</v>
       </c>
-      <c r="L9" s="42">
+      <c r="L9" s="32">
         <v>0.91228100000000001</v>
       </c>
-      <c r="M9" s="26"/>
+      <c r="M9" s="21"/>
     </row>
     <row r="10" spans="2:18" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="1">
         <v>0.6</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="22">
         <v>0.90200000000000002</v>
       </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="16">
+      <c r="F10" s="48"/>
+      <c r="G10" s="13">
         <v>20</v>
       </c>
-      <c r="H10" s="43">
+      <c r="H10" s="33">
         <v>0.95488700000000004</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="33">
         <v>0.94987500000000002</v>
       </c>
-      <c r="J10" s="43">
+      <c r="J10" s="33">
         <v>0.94987500000000002</v>
       </c>
-      <c r="K10" s="43">
+      <c r="K10" s="33">
         <v>0.94736799999999999</v>
       </c>
-      <c r="L10" s="44">
+      <c r="L10" s="34">
         <v>0.91478700000000002</v>
       </c>
-      <c r="M10" s="26"/>
+      <c r="M10" s="21"/>
     </row>
     <row r="11" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="57"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="1">
         <v>0.7</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="22">
         <v>0.91</v>
       </c>
-      <c r="M11" s="26"/>
+      <c r="M11" s="21"/>
     </row>
     <row r="12" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="57"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="1">
         <v>0.8</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="22">
         <v>0.92700000000000005</v>
       </c>
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="2:18" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
-      <c r="C13" s="16">
+      <c r="B13" s="48"/>
+      <c r="C13" s="13">
         <v>0.9</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="24">
         <v>0.91700000000000004</v>
       </c>
-      <c r="F13" s="46"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
+      <c r="F13" s="36"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
     </row>
     <row r="14" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="46"/>
-      <c r="D14" s="26"/>
-      <c r="F14" s="46"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="26"/>
+      <c r="B14" s="36"/>
+      <c r="D14" s="21"/>
+      <c r="F14" s="36"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="21"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="46"/>
-      <c r="D15" s="26"/>
-      <c r="F15" s="46"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="26"/>
+      <c r="B15" s="36"/>
+      <c r="D15" s="21"/>
+      <c r="F15" s="36"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="21"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="46"/>
-      <c r="D16" s="26"/>
-      <c r="F16" s="46"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="52"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="26"/>
+      <c r="B16" s="36"/>
+      <c r="D16" s="21"/>
+      <c r="F16" s="36"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="21"/>
     </row>
     <row r="17" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="46"/>
-      <c r="D17" s="26"/>
-      <c r="F17" s="46"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
-      <c r="J17" s="52"/>
-      <c r="K17" s="52"/>
-      <c r="L17" s="52"/>
+      <c r="B17" s="36"/>
+      <c r="D17" s="21"/>
+      <c r="F17" s="36"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
     </row>
     <row r="18" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="46"/>
-      <c r="D18" s="26"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
+      <c r="B18" s="36"/>
+      <c r="D18" s="21"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
     </row>
     <row r="20" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="55"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="52"/>
-      <c r="K20" s="52"/>
-      <c r="L20" s="52"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
     </row>
     <row r="21" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="55"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+      <c r="L21" s="44"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="F22" s="55"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="52"/>
-      <c r="J22" s="52"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D23" s="46"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="53"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
+      <c r="D23" s="36"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
     </row>
     <row r="24" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D24" s="46"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="53"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-      <c r="L24" s="52"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
+      <c r="D24" s="36"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D25" s="46"/>
-      <c r="F25" s="26"/>
-      <c r="K25" s="46"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
+      <c r="D25" s="36"/>
+      <c r="F25" s="21"/>
+      <c r="K25" s="36"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D26" s="46"/>
-      <c r="F26" s="26"/>
-      <c r="K26" s="46"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
-      <c r="Q26" s="26"/>
-      <c r="R26" s="26"/>
+      <c r="D26" s="36"/>
+      <c r="F26" s="21"/>
+      <c r="K26" s="36"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D27" s="46"/>
-      <c r="F27" s="26"/>
+      <c r="D27" s="36"/>
+      <c r="F27" s="21"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D28" s="46"/>
-      <c r="F28" s="26"/>
+      <c r="D28" s="36"/>
+      <c r="F28" s="21"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D29" s="46"/>
-      <c r="F29" s="26"/>
+      <c r="D29" s="36"/>
+      <c r="F29" s="21"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D30" s="46"/>
-      <c r="F30" s="26"/>
+      <c r="D30" s="36"/>
+      <c r="F30" s="21"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D31" s="46"/>
-      <c r="F31" s="26"/>
+      <c r="D31" s="36"/>
+      <c r="F31" s="21"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D32" s="46"/>
-      <c r="F32" s="26"/>
+      <c r="D32" s="36"/>
+      <c r="F32" s="21"/>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D33" s="46"/>
-      <c r="F33" s="26"/>
+      <c r="D33" s="36"/>
+      <c r="F33" s="21"/>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D34" s="46"/>
-      <c r="F34" s="26"/>
+      <c r="D34" s="36"/>
+      <c r="F34" s="21"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D35" s="46"/>
-      <c r="F35" s="26"/>
+      <c r="D35" s="36"/>
+      <c r="F35" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1556,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F86A2A-D998-CC47-8A5B-54DB70D4D65B}">
   <dimension ref="B1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1586,169 +1537,173 @@
       <c r="L1" s="9"/>
     </row>
     <row r="2" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="72"/>
+      <c r="B2" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="56"/>
       <c r="L2" s="9"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="73" t="s">
+      <c r="B3" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="74"/>
-      <c r="J3" s="77"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="61"/>
       <c r="L3" s="9"/>
     </row>
     <row r="4" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="49"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
+      <c r="B4" s="39"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
       <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="11" t="s">
         <v>15</v>
       </c>
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="63"/>
+      <c r="F5" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="68">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="64"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="70">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I6" s="70"/>
+      <c r="J6" s="71"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="64"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="68">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="70">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="I8" s="70"/>
+      <c r="J8" s="71"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="I9" s="68"/>
+      <c r="J9" s="69"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="79"/>
-      <c r="F5" s="67" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="81">
-        <v>0.64200000000000002</v>
-      </c>
-      <c r="I5" s="81"/>
-      <c r="J5" s="82"/>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D6" s="68"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="83">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="I6" s="83"/>
-      <c r="J6" s="84"/>
-      <c r="L6" s="9"/>
-    </row>
-    <row r="7" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="68"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="67" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="81">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="I7" s="81"/>
-      <c r="J7" s="82"/>
-      <c r="L7" s="9"/>
-    </row>
-    <row r="8" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="68"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="83">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="I8" s="83"/>
-      <c r="J8" s="84"/>
-      <c r="L8" s="9"/>
-    </row>
-    <row r="9" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="68"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="67" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="81">
-        <v>0.87</v>
-      </c>
-      <c r="I9" s="81"/>
-      <c r="J9" s="82"/>
-      <c r="L9" s="9"/>
-    </row>
-    <row r="10" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="68"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="83">
+      <c r="H10" s="70">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I10" s="83"/>
-      <c r="J10" s="84"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="71"/>
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="67" t="s">
+      <c r="E11" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="34"/>
-      <c r="G11" s="23" t="s">
+      <c r="F11" s="28"/>
+      <c r="G11" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="50">
+      <c r="H11" s="40">
         <v>0.436</v>
       </c>
-      <c r="I11" s="50"/>
-      <c r="J11" s="51"/>
+      <c r="I11" s="40">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="J11" s="41">
+        <v>0.79900000000000004</v>
+      </c>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="65"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68" t="s">
+      <c r="D12" s="73"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64" t="s">
         <v>9</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1757,112 +1712,140 @@
       <c r="H12" s="5">
         <v>0.54400000000000004</v>
       </c>
-      <c r="I12" s="5"/>
-      <c r="J12" s="15"/>
+      <c r="I12" s="5">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0.77200000000000002</v>
+      </c>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D13" s="65"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
       <c r="G13" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H13" s="5">
         <v>0.50600000000000001</v>
       </c>
-      <c r="I13" s="5"/>
-      <c r="J13" s="15"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
+      <c r="I13" s="5">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="J13" s="12">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
     </row>
     <row r="14" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="65"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
       <c r="G14" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H14" s="5">
         <v>0.47599999999999998</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="15"/>
+      <c r="I14" s="5">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0.752</v>
+      </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
     </row>
     <row r="15" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="65"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="67" t="s">
+      <c r="D15" s="73"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="50">
+      <c r="H15" s="40">
         <v>0.622</v>
       </c>
-      <c r="I15" s="50"/>
-      <c r="J15" s="51"/>
+      <c r="I15" s="40">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="J15" s="41">
+        <v>0.81699999999999995</v>
+      </c>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="65"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
+      <c r="D16" s="73"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
       <c r="G16" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H16" s="5">
         <v>0.54900000000000004</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="15"/>
+      <c r="I16" s="5">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0.86499999999999999</v>
+      </c>
       <c r="L16" s="6"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
     </row>
     <row r="17" spans="4:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="65"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="17">
+      <c r="D17" s="73"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="67"/>
+      <c r="G17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="14">
         <v>0.56599999999999995</v>
       </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="18"/>
+      <c r="I17" s="14">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="J17" s="15">
+        <v>0.92700000000000005</v>
+      </c>
       <c r="L17" s="6"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
     </row>
     <row r="18" spans="4:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="65"/>
-      <c r="E18" s="64" t="s">
+      <c r="D18" s="73"/>
+      <c r="E18" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="23" t="s">
+      <c r="F18" s="28"/>
+      <c r="G18" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="50">
+      <c r="H18" s="40">
         <v>0.41399999999999998</v>
       </c>
-      <c r="I18" s="50"/>
-      <c r="J18" s="51"/>
+      <c r="I18" s="40">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="J18" s="41">
+        <v>0.83499999999999996</v>
+      </c>
       <c r="L18" s="6"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
     </row>
     <row r="19" spans="4:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="68" t="s">
+      <c r="D19" s="73"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="64" t="s">
         <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -1871,90 +1854,114 @@
       <c r="H19" s="5">
         <v>0.38300000000000001</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="15"/>
+      <c r="I19" s="5">
+        <v>0.629</v>
+      </c>
+      <c r="J19" s="12">
+        <v>0.82199999999999995</v>
+      </c>
       <c r="L19" s="6"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
     </row>
     <row r="20" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="68"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="64"/>
       <c r="G20" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H20" s="5">
         <v>0.39100000000000001</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="15"/>
+      <c r="I20" s="5">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="J20" s="12">
+        <v>0.82699999999999996</v>
+      </c>
       <c r="L20" s="6"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
     </row>
     <row r="21" spans="4:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="68"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="64"/>
       <c r="G21" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H21" s="5">
         <v>0.373</v>
       </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="15"/>
+      <c r="I21" s="5">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="J21" s="12">
+        <v>0.76200000000000001</v>
+      </c>
       <c r="L21" s="6"/>
       <c r="M21" s="5"/>
       <c r="N21" s="5"/>
     </row>
     <row r="22" spans="4:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="67" t="s">
+      <c r="D22" s="73"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="50">
+      <c r="H22" s="40">
         <v>0.49099999999999999</v>
       </c>
-      <c r="I22" s="50"/>
-      <c r="J22" s="51"/>
+      <c r="I22" s="40">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="J22" s="41">
+        <v>0.83499999999999996</v>
+      </c>
       <c r="L22" s="6"/>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
     </row>
     <row r="23" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="68"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
       <c r="G23" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H23" s="5">
         <v>0.45600000000000002</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="15"/>
+      <c r="I23" s="5">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="J23" s="12">
+        <v>0.91</v>
+      </c>
       <c r="L23" s="6"/>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
     </row>
     <row r="24" spans="4:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="17">
+      <c r="D24" s="74"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="14">
         <v>0.46600000000000003</v>
       </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="18"/>
+      <c r="I24" s="14">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="J24" s="15">
+        <v>0.96</v>
+      </c>
       <c r="L24" s="6"/>
       <c r="M24" s="5"/>
       <c r="N24" s="5"/>
@@ -2012,6 +2019,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D11:D24"/>
+    <mergeCell ref="E11:E17"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E18:E24"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F22:F24"/>
     <mergeCell ref="D2:J2"/>
     <mergeCell ref="D3:G4"/>
     <mergeCell ref="H3:J3"/>
@@ -2025,26 +2039,7 @@
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="H9:J9"/>
     <mergeCell ref="H10:J10"/>
-    <mergeCell ref="D11:D24"/>
-    <mergeCell ref="E11:E17"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="E18:E24"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F22:F24"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1 J1">
-    <cfRule type="colorScale" priority="48">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FFFCFCFF"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I1">
     <cfRule type="colorScale" priority="47">
       <colorScale>
@@ -2059,6 +2054,18 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="I11:I24">
     <cfRule type="colorScale" priority="135">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1 H1">
+    <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2111,11 +2118,952 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="C1:X15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B03C0B-9DE5-2F4B-9C2D-1DAFD1F29915}">
+  <dimension ref="B1:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="5" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="56"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="58"/>
+      <c r="J3" s="61"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="39"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="63"/>
+      <c r="F5" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="68">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="64"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="70">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I6" s="70"/>
+      <c r="J6" s="71"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="64"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="68">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="70">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="I8" s="70"/>
+      <c r="J8" s="71"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="I9" s="68"/>
+      <c r="J9" s="69"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="70">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="I10" s="70"/>
+      <c r="J10" s="71"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="40">
+        <v>0.622</v>
+      </c>
+      <c r="I11" s="40">
+        <v>0.77700000000000002</v>
+      </c>
+      <c r="J11" s="41">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+    </row>
+    <row r="13" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="14">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="I13" s="14">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="J13" s="15">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+    </row>
+    <row r="14" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="73"/>
+      <c r="E14" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="40">
+        <v>0.49099999999999999</v>
+      </c>
+      <c r="I14" s="40">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="J14" s="41">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="J15" s="12">
+        <v>0.91</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="I16" s="14">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="J16" s="15">
+        <v>0.96</v>
+      </c>
+      <c r="L16" s="6"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L17" s="6"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L18" s="6"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L19" s="6"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="D3:G4"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="D5:E10"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I1">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1 H1">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M14:M28">
+    <cfRule type="colorScale" priority="150">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N14:N28 M11:N12">
+    <cfRule type="colorScale" priority="151">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:I16">
+    <cfRule type="colorScale" priority="153">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:J16 I5:J6 H5:H16">
+    <cfRule type="colorScale" priority="155">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0620405F-A982-AA41-BD9F-E7AE73492AEE}">
+  <dimension ref="B1:N30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="5" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="56"/>
+      <c r="L2" s="9"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="58"/>
+      <c r="J3" s="61"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="39"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="63"/>
+      <c r="F5" s="66" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="68">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="I5" s="68"/>
+      <c r="J5" s="69"/>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="64"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="70">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I6" s="70"/>
+      <c r="J6" s="71"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="64"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="68">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I7" s="68"/>
+      <c r="J7" s="69"/>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="70">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="I8" s="70"/>
+      <c r="J8" s="71"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D9" s="64"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="68">
+        <v>0.87</v>
+      </c>
+      <c r="I9" s="68"/>
+      <c r="J9" s="69"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="2:14" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="64"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="70">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="I10" s="70"/>
+      <c r="J10" s="71"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="72" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="28"/>
+      <c r="G11" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="40">
+        <v>0.436</v>
+      </c>
+      <c r="I11" s="40">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="J11" s="41">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="J12" s="12">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="J13" s="12">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+    </row>
+    <row r="14" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="I14" s="5">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0.752</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+    </row>
+    <row r="15" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="73"/>
+      <c r="E15" s="72" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="40">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="I15" s="40">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="J15" s="41">
+        <v>0.83499999999999996</v>
+      </c>
+      <c r="L15" s="6"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+    </row>
+    <row r="16" spans="2:14" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="73"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="64" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="75" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="76">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="I16" s="76">
+        <v>0.629</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="L16" s="6"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="76">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="I17" s="76">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L17" s="6"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+    </row>
+    <row r="18" spans="4:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="14">
+        <v>0.373</v>
+      </c>
+      <c r="I18" s="14">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="J18" s="15">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="L18" s="6"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="L19" s="6"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="L20" s="6"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="L21" s="6"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="D11:D18"/>
+    <mergeCell ref="E11:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="E15:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="D3:G4"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="D5:E10"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H7:J7"/>
+    <mergeCell ref="H8:J8"/>
+  </mergeCells>
+  <conditionalFormatting sqref="I1">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1 H1">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M18:M30">
+    <cfRule type="colorScale" priority="142">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N18:N30">
+    <cfRule type="colorScale" priority="144">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11:I18">
+    <cfRule type="colorScale" priority="145">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J11:J18 I5:J6 H5:H18">
+    <cfRule type="colorScale" priority="147">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFCFCFF"/>
+        <color theme="6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
+  <dimension ref="B1:X23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2141,7 +3089,7 @@
     <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="9"/>
@@ -2163,21 +3111,23 @@
       <c r="W1" s="5"/>
       <c r="X1" s="5"/>
     </row>
-    <row r="2" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
@@ -2185,21 +3135,23 @@
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
     </row>
-    <row r="3" spans="3:24" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
@@ -2207,23 +3159,23 @@
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
     </row>
-    <row r="4" spans="3:24" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="6"/>
-      <c r="D4" s="70" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="72"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
@@ -2231,37 +3183,23 @@
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
     </row>
-    <row r="5" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="C5" s="6"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
@@ -2269,32 +3207,23 @@
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
     </row>
-    <row r="6" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D6" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="63">
-        <v>1</v>
-      </c>
-      <c r="F6" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="85">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="4">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="K6" s="14">
-        <v>0.94899999999999995</v>
-      </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="14"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
+    <row r="6" spans="2:24" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
       <c r="T6" s="2"/>
@@ -2302,26 +3231,23 @@
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
     </row>
-    <row r="7" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D7" s="68"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G7" s="85"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="4">
-        <v>0.91300000000000003</v>
-      </c>
-      <c r="K7" s="14">
-        <v>0.95</v>
-      </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="14"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
@@ -2329,30 +3255,23 @@
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
     </row>
-    <row r="8" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D8" s="68"/>
-      <c r="E8" s="63">
-        <v>2</v>
-      </c>
-      <c r="F8" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="85">
-        <v>0.90800000000000003</v>
-      </c>
-      <c r="H8" s="38"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="4">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="K8" s="14">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="14"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
@@ -2360,26 +3279,23 @@
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
     </row>
-    <row r="9" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D9" s="68"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="85"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="4">
-        <v>0.91400000000000003</v>
-      </c>
-      <c r="K9" s="14">
-        <v>0.95</v>
-      </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="14"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
@@ -2387,30 +3303,23 @@
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
     </row>
-    <row r="10" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D10" s="68"/>
-      <c r="E10" s="63">
-        <v>5</v>
-      </c>
-      <c r="F10" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="85">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="H10" s="38"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="4">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="K10" s="14">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="14"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
@@ -2418,26 +3327,23 @@
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
     </row>
-    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D11" s="68"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="85"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="4">
-        <v>0.91800000000000004</v>
-      </c>
-      <c r="K11" s="14">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="14"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
@@ -2445,30 +3351,23 @@
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
     </row>
-    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D12" s="68"/>
-      <c r="E12" s="63">
-        <v>10</v>
-      </c>
-      <c r="F12" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="85">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="H12" s="38"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="K12" s="14">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="14"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
@@ -2476,23 +3375,23 @@
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
     </row>
-    <row r="13" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D13" s="68"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="85"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="4">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="K13" s="14">
-        <v>0.95199999999999996</v>
-      </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="14"/>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
@@ -2500,27 +3399,23 @@
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
     </row>
-    <row r="14" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="D14" s="68"/>
-      <c r="E14" s="63">
-        <v>20</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="85">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="H14" s="38"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="4">
-        <v>0.94099999999999995</v>
-      </c>
-      <c r="K14" s="14">
-        <v>0.94</v>
-      </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="14"/>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
@@ -2528,40 +3423,170 @@
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
     </row>
-    <row r="15" spans="3:24" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="69"/>
-      <c r="E15" s="86"/>
-      <c r="F15" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="83"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="21">
-        <v>0.91200000000000003</v>
-      </c>
-      <c r="K15" s="22">
-        <v>0.94699999999999995</v>
-      </c>
-      <c r="L15" s="21"/>
-      <c r="M15" s="22"/>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="D4:M4"/>
-    <mergeCell ref="D6:D15"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G10:G11"/>
-  </mergeCells>
-  <conditionalFormatting sqref="G1:J3">
+  <conditionalFormatting sqref="G1:J1">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -2573,20 +3598,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G6:M15">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color theme="2"/>
-        <color theme="6"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P1:P12">
-    <cfRule type="colorScale" priority="38">
+  <conditionalFormatting sqref="O1 Q1">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2597,8 +3610,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q1:Q12 O1:O12">
-    <cfRule type="colorScale" priority="39">
+  <conditionalFormatting sqref="P1">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
added union correction results
</commit_message>
<xml_diff>
--- a/misc/union_results.xlsx
+++ b/misc/union_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9FE231-C3A1-FB4F-8E02-510B18E8AC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F27061-8C6B-3847-90D0-F770A8793F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="8160" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="llm (hint)" sheetId="14" r:id="rId2"/>
     <sheet name="llm (values)" sheetId="12" r:id="rId3"/>
     <sheet name="llm-correction" sheetId="9" r:id="rId4"/>
-    <sheet name="llm (all)" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>Zero-Shot</t>
   </si>
@@ -400,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,6 +539,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -570,49 +593,46 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -630,58 +650,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1022,7 +991,7 @@
   <dimension ref="B2:T34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1053,15 +1022,15 @@
       <c r="D3" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="50" t="s">
+      <c r="F3" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="52"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="60"/>
       <c r="N3" s="10"/>
       <c r="O3" s="12" t="s">
         <v>13</v>
@@ -1077,7 +1046,7 @@
       </c>
     </row>
     <row r="4" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="55" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="12">
@@ -1086,15 +1055,15 @@
       <c r="D4" s="29">
         <v>0.85699999999999998</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51" t="s">
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="52"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="60"/>
       <c r="N4" s="19" t="s">
         <v>35</v>
       </c>
@@ -1116,15 +1085,15 @@
       </c>
     </row>
     <row r="5" spans="2:18" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="48"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="16">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="54"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
       <c r="H5" s="1">
         <v>0.5</v>
       </c>
@@ -1162,14 +1131,14 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="48"/>
+      <c r="B6" s="56"/>
       <c r="C6" s="1">
         <v>3</v>
       </c>
       <c r="D6" s="16">
         <v>0.85699999999999998</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="56" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="1">
@@ -1198,14 +1167,14 @@
       <c r="R6" s="7"/>
     </row>
     <row r="7" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="48"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="16">
         <v>0.84199999999999997</v>
       </c>
-      <c r="F7" s="48"/>
+      <c r="F7" s="56"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -1232,16 +1201,16 @@
       <c r="R7" s="15"/>
     </row>
     <row r="8" spans="2:18" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="49"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="9">
         <v>5</v>
       </c>
       <c r="D8" s="18">
         <v>0.84199999999999997</v>
       </c>
-      <c r="F8" s="48"/>
+      <c r="F8" s="56"/>
       <c r="G8" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H8" s="34">
         <v>0.96240599999999998</v>
@@ -1266,7 +1235,7 @@
       <c r="R8" s="15"/>
     </row>
     <row r="9" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="12">
@@ -1275,9 +1244,9 @@
       <c r="D9" s="29">
         <v>0.88200000000000001</v>
       </c>
-      <c r="F9" s="48"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H9" s="34">
         <v>0.95238100000000003</v>
@@ -1297,16 +1266,16 @@
       <c r="M9" s="15"/>
     </row>
     <row r="10" spans="2:18" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="48"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="1">
         <v>0.6</v>
       </c>
       <c r="D10" s="16">
         <v>0.90200000000000002</v>
       </c>
-      <c r="F10" s="49"/>
+      <c r="F10" s="57"/>
       <c r="G10" s="9">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="H10" s="27">
         <v>0.95488700000000004</v>
@@ -1326,7 +1295,7 @@
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="48"/>
+      <c r="B11" s="56"/>
       <c r="C11" s="1">
         <v>0.7</v>
       </c>
@@ -1336,7 +1305,7 @@
       <c r="M11" s="15"/>
     </row>
     <row r="12" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="48"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="1">
         <v>0.8</v>
       </c>
@@ -1346,7 +1315,7 @@
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="2:18" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="49"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="9">
         <v>0.9</v>
       </c>
@@ -1619,7 +1588,7 @@
   <dimension ref="B1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1653,27 +1622,27 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="33"/>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56" t="s">
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="59"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="67"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="42" t="s">
         <v>37</v>
       </c>
@@ -1695,118 +1664,118 @@
       <c r="B4" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="62" t="s">
+      <c r="E4" s="69"/>
+      <c r="F4" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="84" t="s">
+      <c r="G4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="85">
+      <c r="H4" s="72">
         <v>0.84199999999999997</v>
       </c>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="71"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="73"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="65"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="71"/>
       <c r="G5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="68">
+      <c r="H5" s="74">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="69"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="75"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="33"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="64" t="s">
+      <c r="D6" s="70"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="76" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="66">
+      <c r="H6" s="77">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="67"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="78"/>
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="65"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="74">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="69"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="75"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="62"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="64" t="s">
+      <c r="D8" s="70"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="76" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="66">
+      <c r="H8" s="77">
         <v>0.87</v>
       </c>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="67"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="78"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="62"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="62"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
       <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="70">
+      <c r="H9" s="72">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="71"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="73"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="76" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="22"/>
@@ -1816,170 +1785,202 @@
       <c r="H10" s="38">
         <v>0.436</v>
       </c>
-      <c r="I10" s="38"/>
+      <c r="I10" s="38">
+        <v>0.36599999999999999</v>
+      </c>
       <c r="J10" s="38">
         <v>0.45400000000000001</v>
       </c>
       <c r="K10" s="38">
         <v>0.79900000000000004</v>
       </c>
-      <c r="L10" s="39"/>
+      <c r="L10" s="39">
+        <v>0.81699999999999995</v>
+      </c>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="73"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62" t="s">
+      <c r="D11" s="80"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="88" t="s">
+      <c r="G11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="89">
+      <c r="H11" s="2">
         <v>0.54400000000000004</v>
       </c>
-      <c r="I11" s="89"/>
-      <c r="J11" s="89">
+      <c r="I11" s="2">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="J11" s="2">
         <v>0.58599999999999997</v>
       </c>
-      <c r="K11" s="89">
+      <c r="K11" s="2">
         <v>0.77200000000000002</v>
       </c>
-      <c r="L11" s="43"/>
+      <c r="L11" s="43">
+        <v>0.78400000000000003</v>
+      </c>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D12" s="73"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="88" t="s">
+      <c r="D12" s="80"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="89">
+      <c r="H12" s="2">
         <v>0.50600000000000001</v>
       </c>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89">
+      <c r="I12" s="2">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="J12" s="2">
         <v>0.48099999999999998</v>
       </c>
-      <c r="K12" s="89">
+      <c r="K12" s="2">
         <v>0.85199999999999998</v>
       </c>
-      <c r="L12" s="43"/>
+      <c r="L12" s="43">
+        <v>0.77700000000000002</v>
+      </c>
       <c r="O12" s="21"/>
       <c r="P12" s="21"/>
     </row>
     <row r="13" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="73"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="65"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="71"/>
       <c r="G13" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="40">
         <v>0.47599999999999998</v>
       </c>
-      <c r="I13" s="40"/>
+      <c r="I13" s="40">
+        <v>0.624</v>
+      </c>
       <c r="J13" s="40">
         <v>0.41399999999999998</v>
       </c>
       <c r="K13" s="40">
         <v>0.752</v>
       </c>
-      <c r="L13" s="41"/>
+      <c r="L13" s="41">
+        <v>0.52400000000000002</v>
+      </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
     </row>
     <row r="14" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="73"/>
-      <c r="E14" s="64" t="s">
+      <c r="D14" s="80"/>
+      <c r="E14" s="76" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="46"/>
-      <c r="G14" s="88" t="s">
+      <c r="G14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H14" s="89">
+      <c r="H14" s="2">
         <v>0.41399999999999998</v>
       </c>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89">
+      <c r="I14" s="2">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="J14" s="2">
         <v>0.52100000000000002</v>
       </c>
-      <c r="K14" s="89">
+      <c r="K14" s="2">
         <v>0.83499999999999996</v>
       </c>
-      <c r="L14" s="43"/>
+      <c r="L14" s="43">
+        <v>0.80200000000000005</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="73"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62" t="s">
+      <c r="D15" s="80"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="88" t="s">
+      <c r="G15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="89">
+      <c r="H15" s="2">
         <v>0.38300000000000001</v>
       </c>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89">
+      <c r="I15" s="2">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="J15" s="2">
         <v>0.629</v>
       </c>
-      <c r="K15" s="89">
+      <c r="K15" s="2">
         <v>0.82199999999999995</v>
       </c>
-      <c r="L15" s="43"/>
+      <c r="L15" s="43">
+        <v>0.77700000000000002</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D16" s="73"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="88" t="s">
+      <c r="D16" s="80"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H16" s="89">
+      <c r="H16" s="2">
         <v>0.39100000000000001</v>
       </c>
-      <c r="I16" s="89"/>
-      <c r="J16" s="89">
+      <c r="I16" s="2">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="J16" s="2">
         <v>0.64700000000000002</v>
       </c>
-      <c r="K16" s="89">
+      <c r="K16" s="2">
         <v>0.82699999999999996</v>
       </c>
-      <c r="L16" s="43"/>
+      <c r="L16" s="43">
+        <v>0.77900000000000003</v>
+      </c>
       <c r="N16" s="4"/>
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="74"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="71"/>
       <c r="G17" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H17" s="40">
         <v>0.373</v>
       </c>
-      <c r="I17" s="40"/>
+      <c r="I17" s="40">
+        <v>0.42399999999999999</v>
+      </c>
       <c r="J17" s="40">
         <v>0.56399999999999995</v>
       </c>
       <c r="K17" s="40">
         <v>0.76200000000000001</v>
       </c>
-      <c r="L17" s="41"/>
+      <c r="L17" s="41">
+        <v>0.81499999999999995</v>
+      </c>
       <c r="N17" s="4"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
@@ -2077,7 +2078,7 @@
   <dimension ref="B1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2111,27 +2112,27 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="33"/>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56" t="s">
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="59"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="67"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="42" t="s">
         <v>37</v>
       </c>
@@ -2150,124 +2151,124 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="62" t="s">
+      <c r="E4" s="69"/>
+      <c r="F4" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="84" t="s">
+      <c r="G4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="85">
+      <c r="H4" s="72">
         <v>0.84199999999999997</v>
       </c>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="71"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="73"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="65"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="71"/>
       <c r="G5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="68">
+      <c r="H5" s="74">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="69"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="75"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="33"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="64" t="s">
+      <c r="D6" s="70"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="76" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="66">
+      <c r="H6" s="77">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="66"/>
-      <c r="L6" s="67"/>
+      <c r="I6" s="77"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="77"/>
+      <c r="L6" s="78"/>
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="65"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="71"/>
       <c r="G7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="68">
+      <c r="H7" s="74">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="69"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="75"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="62"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="64" t="s">
+      <c r="D8" s="70"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="76" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="66">
+      <c r="H8" s="77">
         <v>0.87</v>
       </c>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="67"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="78"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="62"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="62"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="70"/>
       <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="70">
+      <c r="H9" s="72">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="71"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="73"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="76" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="12" t="s">
@@ -2276,127 +2277,151 @@
       <c r="H10" s="38">
         <v>0.622</v>
       </c>
-      <c r="I10" s="38"/>
+      <c r="I10" s="38">
+        <v>0.63900000000000001</v>
+      </c>
       <c r="J10" s="38">
         <v>0.77700000000000002</v>
       </c>
       <c r="K10" s="38">
         <v>0.81699999999999995</v>
       </c>
-      <c r="L10" s="39"/>
+      <c r="L10" s="39">
+        <v>0.83699999999999997</v>
+      </c>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D11" s="73"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="88" t="s">
+      <c r="D11" s="80"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="89">
+      <c r="H11" s="2">
         <v>0.54900000000000004</v>
       </c>
-      <c r="I11" s="89"/>
-      <c r="J11" s="89">
+      <c r="I11" s="2">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="J11" s="2">
         <v>0.74399999999999999</v>
       </c>
-      <c r="K11" s="89">
+      <c r="K11" s="2">
         <v>0.86499999999999999</v>
       </c>
-      <c r="L11" s="43"/>
+      <c r="L11" s="43">
+        <v>0.86199999999999999</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="8"/>
       <c r="P11" s="8"/>
     </row>
     <row r="12" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="73"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="65"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
       <c r="G12" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="40">
         <v>0.56599999999999995</v>
       </c>
-      <c r="I12" s="40"/>
+      <c r="I12" s="40">
+        <v>0.63200000000000001</v>
+      </c>
       <c r="J12" s="40">
         <v>0.79700000000000004</v>
       </c>
       <c r="K12" s="40">
         <v>0.92700000000000005</v>
       </c>
-      <c r="L12" s="41"/>
+      <c r="L12" s="41">
+        <v>0.95499999999999996</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
     </row>
     <row r="13" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="73"/>
-      <c r="E13" s="62" t="s">
+      <c r="D13" s="80"/>
+      <c r="E13" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="62" t="s">
+      <c r="F13" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="88" t="s">
+      <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="89">
+      <c r="H13" s="2">
         <v>0.49099999999999999</v>
       </c>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89">
+      <c r="I13" s="2">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="J13" s="2">
         <v>0.76900000000000002</v>
       </c>
-      <c r="K13" s="89">
+      <c r="K13" s="2">
         <v>0.83499999999999996</v>
       </c>
-      <c r="L13" s="43"/>
+      <c r="L13" s="43">
+        <v>0.82</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D14" s="73"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="88" t="s">
+      <c r="D14" s="80"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="89">
+      <c r="H14" s="2">
         <v>0.45600000000000002</v>
       </c>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89">
+      <c r="I14" s="2">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="J14" s="2">
         <v>0.88200000000000001</v>
       </c>
-      <c r="K14" s="89">
+      <c r="K14" s="2">
         <v>0.91</v>
       </c>
-      <c r="L14" s="43"/>
+      <c r="L14" s="43">
+        <v>0.89</v>
+      </c>
       <c r="N14" s="4"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="74"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
       <c r="G15" s="9" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="40">
         <v>0.46600000000000003</v>
       </c>
-      <c r="I15" s="40"/>
+      <c r="I15" s="40">
+        <v>0.77900000000000003</v>
+      </c>
       <c r="J15" s="40">
         <v>0.80500000000000005</v>
       </c>
       <c r="K15" s="40">
         <v>0.96</v>
       </c>
-      <c r="L15" s="41"/>
+      <c r="L15" s="41">
+        <v>0.88200000000000001</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
@@ -2494,7 +2519,7 @@
   <dimension ref="B1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2507,7 +2532,7 @@
     <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -2541,18 +2566,18 @@
     </row>
     <row r="2" spans="2:17" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="77" t="s">
+      <c r="C2" s="82"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="77" t="s">
+      <c r="F2" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="77" t="s">
+      <c r="G2" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="78" t="s">
+      <c r="H2" s="48" t="s">
         <v>38</v>
       </c>
       <c r="I2" s="7"/>
@@ -2567,18 +2592,18 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B3" s="7"/>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="79">
+      <c r="E3" s="49">
         <v>0.84199999999999997</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
-      <c r="H3" s="92"/>
+      <c r="H3" s="13"/>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -2591,16 +2616,14 @@
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="88" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="80">
+      <c r="E4" s="50">
         <v>0.92700000000000005</v>
       </c>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="93"/>
+      <c r="H4" s="14"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -2613,18 +2636,17 @@
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="7"/>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="88" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="80">
+      <c r="E5" s="50">
         <v>0.87</v>
       </c>
-      <c r="F5" s="88"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="93"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="14"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -2637,16 +2659,16 @@
     </row>
     <row r="6" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
-      <c r="C6" s="81"/>
+      <c r="C6" s="84"/>
       <c r="D6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="91">
+      <c r="E6" s="53">
         <v>0.96199999999999997</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="94"/>
+      <c r="H6" s="54"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -2666,573 +2688,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F86A2A-D998-CC47-8A5B-54DB70D4D65B}">
-  <dimension ref="B1:O35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="1"/>
-    <col min="4" max="5" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.1640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="M1" s="7"/>
-    </row>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="33"/>
-      <c r="D2" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="59"/>
-      <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="2:15" ht="41" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="7"/>
-    </row>
-    <row r="4" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="60" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="61"/>
-      <c r="F4" s="64" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="66">
-        <v>0.64200000000000002</v>
-      </c>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="67"/>
-      <c r="M4" s="7"/>
-    </row>
-    <row r="5" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="62"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="68">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="69"/>
-      <c r="M5" s="7"/>
-    </row>
-    <row r="6" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="33"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="66">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="I6" s="66"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="67"/>
-      <c r="M6" s="7"/>
-    </row>
-    <row r="7" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="68">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="I7" s="68"/>
-      <c r="J7" s="68"/>
-      <c r="K7" s="69"/>
-      <c r="M7" s="7"/>
-    </row>
-    <row r="8" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="62"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="64" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="66">
-        <v>0.87</v>
-      </c>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="67"/>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="2:15" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="62"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="70">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="71"/>
-      <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="72" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="38">
-        <v>0.436</v>
-      </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="K10" s="39">
-        <v>0.79900000000000004</v>
-      </c>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-    </row>
-    <row r="11" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="73"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2">
-        <v>0.58599999999999997</v>
-      </c>
-      <c r="K11" s="43">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D12" s="73"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.50600000000000001</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2">
-        <v>0.48099999999999998</v>
-      </c>
-      <c r="K12" s="43">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="N12" s="21"/>
-      <c r="O12" s="21"/>
-    </row>
-    <row r="13" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="73"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="40">
-        <v>0.47599999999999998</v>
-      </c>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40">
-        <v>0.41399999999999998</v>
-      </c>
-      <c r="K13" s="41">
-        <v>0.752</v>
-      </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="2:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="73"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="64" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="38">
-        <v>0.622</v>
-      </c>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38">
-        <v>0.77700000000000002</v>
-      </c>
-      <c r="K14" s="39">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="D15" s="73"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2">
-        <v>0.74399999999999999</v>
-      </c>
-      <c r="K15" s="43">
-        <v>0.86499999999999999</v>
-      </c>
-      <c r="M15" s="4"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-    </row>
-    <row r="16" spans="2:15" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="73"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="40">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40">
-        <v>0.79700000000000004</v>
-      </c>
-      <c r="K16" s="41">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="M16" s="4"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-    </row>
-    <row r="17" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="73"/>
-      <c r="E17" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="38">
-        <v>0.41399999999999998</v>
-      </c>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38">
-        <v>0.52100000000000002</v>
-      </c>
-      <c r="K17" s="39">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="M17" s="4"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-    </row>
-    <row r="18" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="73"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2">
-        <v>0.629</v>
-      </c>
-      <c r="K18" s="43">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="M18" s="4"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-    </row>
-    <row r="19" spans="4:15" x14ac:dyDescent="0.2">
-      <c r="D19" s="73"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="K19" s="43">
-        <v>0.82699999999999996</v>
-      </c>
-      <c r="M19" s="4"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-    </row>
-    <row r="20" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="73"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" s="40">
-        <v>0.373</v>
-      </c>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40">
-        <v>0.56399999999999995</v>
-      </c>
-      <c r="K20" s="41">
-        <v>0.76200000000000001</v>
-      </c>
-      <c r="M20" s="4"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-    </row>
-    <row r="21" spans="4:15" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="73"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0.49099999999999999</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2">
-        <v>0.76900000000000002</v>
-      </c>
-      <c r="K21" s="43">
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="M21" s="4"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-    </row>
-    <row r="22" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D22" s="73"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0.45600000000000002</v>
-      </c>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="K22" s="43">
-        <v>0.91</v>
-      </c>
-      <c r="M22" s="4"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-    </row>
-    <row r="23" spans="4:15" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="74"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H23" s="40">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40">
-        <v>0.80500000000000005</v>
-      </c>
-      <c r="K23" s="41">
-        <v>0.96</v>
-      </c>
-      <c r="M23" s="4"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-    </row>
-    <row r="24" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="M24" s="4"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-    </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="M25" s="4"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="M26" s="4"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-    </row>
-    <row r="32" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
-    </row>
-    <row r="33" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-    </row>
-    <row r="34" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
-    </row>
-    <row r="35" spans="14:15" x14ac:dyDescent="0.25">
-      <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="D10:D23"/>
-    <mergeCell ref="E10:E16"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="E17:E23"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="D4:E9"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-  </mergeCells>
-  <conditionalFormatting sqref="H4:K23">
-    <cfRule type="colorScale" priority="150">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color theme="2" tint="-9.9978637043366805E-2"/>
-        <color theme="6" tint="-0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated union correction results
</commit_message>
<xml_diff>
--- a/misc/union_results.xlsx
+++ b/misc/union_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F27061-8C6B-3847-90D0-F770A8793F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66F8260-3755-CE4C-BA92-BAFF823F5076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="8160" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="8660" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -587,6 +587,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,12 +626,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -626,23 +638,11 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1622,27 +1622,27 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="33"/>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64" t="s">
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="67"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="73"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="42" t="s">
         <v>37</v>
       </c>
@@ -1664,118 +1664,118 @@
       <c r="B4" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70" t="s">
+      <c r="E4" s="75"/>
+      <c r="F4" s="67" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="72">
+      <c r="H4" s="76">
         <v>0.84199999999999997</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="73"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="77"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="71"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="68"/>
       <c r="G5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="74">
+      <c r="H5" s="78">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="79"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="33"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="76" t="s">
+      <c r="D6" s="67"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="66" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="77">
+      <c r="H6" s="80">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="78"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="81"/>
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="70"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="71"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="74">
+      <c r="H7" s="78">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="75"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="79"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="70"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="76" t="s">
+      <c r="D8" s="67"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="66" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="80">
         <v>0.87</v>
       </c>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="78"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="81"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="70"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="72">
+      <c r="H9" s="76">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="77"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="79" t="s">
+      <c r="D10" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="66" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="22"/>
@@ -1801,9 +1801,9 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="80"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70" t="s">
+      <c r="D11" s="64"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67" t="s">
         <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1828,9 +1828,9 @@
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D12" s="80"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
       <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1853,9 +1853,9 @@
       <c r="P12" s="21"/>
     </row>
     <row r="13" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="80"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="71"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="68"/>
       <c r="G13" s="9" t="s">
         <v>24</v>
       </c>
@@ -1878,8 +1878,8 @@
       <c r="P13" s="6"/>
     </row>
     <row r="14" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="80"/>
-      <c r="E14" s="76" t="s">
+      <c r="D14" s="64"/>
+      <c r="E14" s="66" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="46"/>
@@ -1906,9 +1906,9 @@
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="80"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70" t="s">
+      <c r="D15" s="64"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1934,9 +1934,9 @@
       <c r="P15" s="8"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D16" s="80"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
       <c r="G16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1960,9 +1960,9 @@
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="81"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
       <c r="G17" s="9" t="s">
         <v>24</v>
       </c>
@@ -2038,11 +2038,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F15:F17"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E9"/>
@@ -2055,6 +2050,11 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="H9:L9"/>
+    <mergeCell ref="D10:D17"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F15:F17"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L17">
     <cfRule type="colorScale" priority="151">
@@ -2077,7 +2077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B03C0B-9DE5-2F4B-9C2D-1DAFD1F29915}">
   <dimension ref="B1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
@@ -2112,27 +2112,27 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="33"/>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64" t="s">
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="67"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="73"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="42" t="s">
         <v>37</v>
       </c>
@@ -2154,121 +2154,121 @@
       <c r="B4" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70" t="s">
+      <c r="E4" s="75"/>
+      <c r="F4" s="67" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="72">
+      <c r="H4" s="76">
         <v>0.84199999999999997</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="73"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="77"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="71"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="68"/>
       <c r="G5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="74">
+      <c r="H5" s="78">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="79"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="33"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="76" t="s">
+      <c r="D6" s="67"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="66" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="77">
+      <c r="H6" s="80">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="78"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="81"/>
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="70"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="71"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="74">
+      <c r="H7" s="78">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="75"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="79"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="70"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="76" t="s">
+      <c r="D8" s="67"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="66" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="80">
         <v>0.87</v>
       </c>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="78"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="81"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="70"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="72">
+      <c r="H9" s="76">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="77"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="79" t="s">
+      <c r="D10" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="76" t="s">
+      <c r="F10" s="66" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="12" t="s">
@@ -2293,9 +2293,9 @@
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D11" s="80"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
       <c r="G11" s="1" t="s">
         <v>16</v>
       </c>
@@ -2319,9 +2319,9 @@
       <c r="P11" s="8"/>
     </row>
     <row r="12" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="80"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
       <c r="G12" s="9" t="s">
         <v>24</v>
       </c>
@@ -2345,11 +2345,11 @@
       <c r="P12" s="8"/>
     </row>
     <row r="13" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="80"/>
-      <c r="E13" s="70" t="s">
+      <c r="D13" s="64"/>
+      <c r="E13" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="70" t="s">
+      <c r="F13" s="67" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -2375,9 +2375,9 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D14" s="80"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
       <c r="G14" s="1" t="s">
         <v>16</v>
       </c>
@@ -2401,9 +2401,9 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="81"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
       <c r="G15" s="9" t="s">
         <v>24</v>
       </c>
@@ -2479,11 +2479,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E9"/>
@@ -2496,6 +2491,11 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="H9:L9"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L15">
     <cfRule type="colorScale" priority="152">
@@ -2518,8 +2518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
   <dimension ref="B1:Q6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2601,9 +2601,13 @@
       <c r="E3" s="49">
         <v>0.84199999999999997</v>
       </c>
-      <c r="F3" s="12"/>
+      <c r="F3" s="12">
+        <v>0.877</v>
+      </c>
       <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="H3" s="13">
+        <v>0.89700000000000002</v>
+      </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -2623,7 +2627,12 @@
       <c r="E4" s="50">
         <v>0.92700000000000005</v>
       </c>
-      <c r="H4" s="14"/>
+      <c r="F4" s="1">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="H4" s="14">
+        <v>0.93500000000000005</v>
+      </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -2645,8 +2654,13 @@
       <c r="E5" s="50">
         <v>0.87</v>
       </c>
+      <c r="F5" s="1">
+        <v>0.92500000000000004</v>
+      </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="14"/>
+      <c r="H5" s="14">
+        <v>0.94699999999999995</v>
+      </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -2666,9 +2680,13 @@
       <c r="E6" s="53">
         <v>0.96199999999999997</v>
       </c>
-      <c r="F6" s="9"/>
+      <c r="F6" s="9">
+        <v>0.95699999999999996</v>
+      </c>
       <c r="G6" s="9"/>
-      <c r="H6" s="54"/>
+      <c r="H6" s="54">
+        <v>0.94199999999999995</v>
+      </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>

</xml_diff>

<commit_message>
qwen plus correctin results are amazing
</commit_message>
<xml_diff>
--- a/misc/union_results.xlsx
+++ b/misc/union_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6927705-2606-3545-A616-0C615EA8188A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB93A2F-A520-0B44-8752-E5BE63D103A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="8660" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" activeTab="1" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -587,6 +587,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,12 +626,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -626,23 +638,11 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1587,8 +1587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0E853E-51FD-9145-8DA3-30D891509AAC}">
   <dimension ref="B1:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1622,27 +1622,27 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="33"/>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64" t="s">
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="67"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="73"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="42" t="s">
         <v>37</v>
       </c>
@@ -1664,118 +1664,118 @@
       <c r="B4" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70" t="s">
+      <c r="E4" s="75"/>
+      <c r="F4" s="67" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="72">
+      <c r="H4" s="76">
         <v>0.84199999999999997</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="73"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="77"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="71"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="68"/>
       <c r="G5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="74">
+      <c r="H5" s="78">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="79"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="33"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="76" t="s">
+      <c r="D6" s="67"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="66" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="77">
+      <c r="H6" s="80">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="78"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="81"/>
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="70"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="71"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="74">
+      <c r="H7" s="78">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="75"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="79"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="70"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="76" t="s">
+      <c r="D8" s="67"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="66" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="80">
         <v>0.87</v>
       </c>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="78"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="81"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="70"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="72">
+      <c r="H9" s="76">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="77"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="79" t="s">
+      <c r="D10" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="66" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="22"/>
@@ -1801,9 +1801,9 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="80"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70" t="s">
+      <c r="D11" s="64"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67" t="s">
         <v>8</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1828,9 +1828,9 @@
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D12" s="80"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
       <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
@@ -1853,9 +1853,9 @@
       <c r="P12" s="21"/>
     </row>
     <row r="13" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="80"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="71"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="68"/>
       <c r="G13" s="9" t="s">
         <v>24</v>
       </c>
@@ -1878,8 +1878,8 @@
       <c r="P13" s="6"/>
     </row>
     <row r="14" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="80"/>
-      <c r="E14" s="76" t="s">
+      <c r="D14" s="64"/>
+      <c r="E14" s="66" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="46"/>
@@ -1906,9 +1906,9 @@
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="80"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70" t="s">
+      <c r="D15" s="64"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67" t="s">
         <v>8</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1934,9 +1934,9 @@
       <c r="P15" s="8"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D16" s="80"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="67"/>
       <c r="G16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1960,9 +1960,9 @@
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="81"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
       <c r="G17" s="9" t="s">
         <v>24</v>
       </c>
@@ -2038,11 +2038,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F15:F17"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E9"/>
@@ -2055,6 +2050,11 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="H9:L9"/>
+    <mergeCell ref="D10:D17"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F15:F17"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L17">
     <cfRule type="colorScale" priority="151">
@@ -2112,27 +2112,27 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="33"/>
-      <c r="D2" s="63" t="s">
+      <c r="D2" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64" t="s">
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="67"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="73"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="33"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="42" t="s">
         <v>37</v>
       </c>
@@ -2154,121 +2154,121 @@
       <c r="B4" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="69"/>
-      <c r="F4" s="70" t="s">
+      <c r="E4" s="75"/>
+      <c r="F4" s="67" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="72">
+      <c r="H4" s="76">
         <v>0.84199999999999997</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="73"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="77"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="70"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="71"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="68"/>
       <c r="G5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="74">
+      <c r="H5" s="78">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="75"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="79"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="33"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="76" t="s">
+      <c r="D6" s="67"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="66" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="77">
+      <c r="H6" s="80">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I6" s="77"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="77"/>
-      <c r="L6" s="78"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="81"/>
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="70"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="71"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="68"/>
       <c r="G7" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="74">
+      <c r="H7" s="78">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="75"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="79"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="70"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="76" t="s">
+      <c r="D8" s="67"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="66" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="77">
+      <c r="H8" s="80">
         <v>0.87</v>
       </c>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="78"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+      <c r="L8" s="81"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="70"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="70"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="72">
+      <c r="H9" s="76">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I9" s="72"/>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="73"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76"/>
+      <c r="L9" s="77"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="79" t="s">
+      <c r="D10" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="76" t="s">
+      <c r="F10" s="66" t="s">
         <v>9</v>
       </c>
       <c r="G10" s="12" t="s">
@@ -2293,9 +2293,9 @@
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D11" s="80"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
       <c r="G11" s="1" t="s">
         <v>16</v>
       </c>
@@ -2319,9 +2319,9 @@
       <c r="P11" s="8"/>
     </row>
     <row r="12" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="80"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
       <c r="G12" s="9" t="s">
         <v>24</v>
       </c>
@@ -2345,11 +2345,11 @@
       <c r="P12" s="8"/>
     </row>
     <row r="13" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="80"/>
-      <c r="E13" s="70" t="s">
+      <c r="D13" s="64"/>
+      <c r="E13" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="70" t="s">
+      <c r="F13" s="67" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -2375,9 +2375,9 @@
       <c r="P13" s="2"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D14" s="80"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
       <c r="G14" s="1" t="s">
         <v>16</v>
       </c>
@@ -2401,9 +2401,9 @@
       <c r="P14" s="2"/>
     </row>
     <row r="15" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="81"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
       <c r="G15" s="9" t="s">
         <v>24</v>
       </c>
@@ -2479,11 +2479,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E9"/>
@@ -2496,6 +2491,11 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="H9:L9"/>
+    <mergeCell ref="D10:D15"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L15">
     <cfRule type="colorScale" priority="152">
@@ -2516,10 +2516,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
-  <dimension ref="B1:Q6"/>
+  <dimension ref="C1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2546,26 +2546,8 @@
     <col min="23" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-    </row>
-    <row r="2" spans="2:17" ht="41" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="7"/>
+    <row r="1" spans="3:8" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:8" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C2" s="82"/>
       <c r="D2" s="83"/>
       <c r="E2" s="47" t="s">
@@ -2580,18 +2562,8 @@
       <c r="H2" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="7"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C3" s="61" t="s">
         <v>35</v>
       </c>
@@ -2610,18 +2582,8 @@
       <c r="H3" s="13">
         <v>0.89700000000000002</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B4" s="7"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C4" s="61"/>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -2638,18 +2600,8 @@
       <c r="H4" s="14">
         <v>0.93500000000000005</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B5" s="7"/>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C5" s="61" t="s">
         <v>11</v>
       </c>
@@ -2668,18 +2620,8 @@
       <c r="H5" s="14">
         <v>0.94699999999999995</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-    </row>
-    <row r="6" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
+    </row>
+    <row r="6" spans="3:8" ht="20" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="84"/>
       <c r="D6" s="9" t="s">
         <v>14</v>
@@ -2690,19 +2632,12 @@
       <c r="F6" s="9">
         <v>0.95699999999999996</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="9">
+        <v>0.96499999999999997</v>
+      </c>
       <c r="H6" s="54">
         <v>0.94199999999999995</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
added cot code for union task
</commit_message>
<xml_diff>
--- a/misc/union_results.xlsx
+++ b/misc/union_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353B6598-AC67-AF46-9601-6486B48E3A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FD70CB-C2BC-7648-9999-F3C763EBF11E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="5380" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -39,13 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
-  <si>
-    <t>Zero-Shot</t>
-  </si>
-  <si>
-    <t>Few-Shot</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="39">
   <si>
     <t>heuristic</t>
   </si>
@@ -159,6 +153,12 @@
   <si>
     <t>4o
 ($2.5/M)</t>
+  </si>
+  <si>
+    <t>ZS (CoT)</t>
+  </si>
+  <si>
+    <t>FS (CoT)</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -464,9 +464,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -536,55 +533,97 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -596,54 +635,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -651,6 +642,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -991,7 +1003,7 @@
   <dimension ref="B2:T34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1013,59 +1025,59 @@
   <sheetData>
     <row r="2" spans="2:18" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:18" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="60"/>
+      <c r="B3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="58"/>
       <c r="N3" s="10"/>
       <c r="O3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="P3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="R3" s="13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="55" t="s">
-        <v>3</v>
+      <c r="B4" s="53" t="s">
+        <v>1</v>
       </c>
       <c r="C4" s="12">
         <v>1</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="28">
         <v>0.85699999999999998</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="60"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="58"/>
       <c r="N4" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O4" s="15">
         <f>MIN($D$4:$D$13)</f>
@@ -1085,15 +1097,15 @@
       </c>
     </row>
     <row r="5" spans="2:18" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="56"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="16">
         <v>0.86699999999999999</v>
       </c>
-      <c r="F5" s="61"/>
-      <c r="G5" s="62"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="60"/>
       <c r="H5" s="1">
         <v>0.5</v>
       </c>
@@ -1111,7 +1123,7 @@
       </c>
       <c r="M5" s="15"/>
       <c r="N5" s="20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="O5" s="17">
         <f>MIN($H$6:$L$10)</f>
@@ -1131,32 +1143,32 @@
       </c>
     </row>
     <row r="6" spans="2:18" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="56"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="1">
         <v>3</v>
       </c>
       <c r="D6" s="16">
         <v>0.85699999999999998</v>
       </c>
-      <c r="F6" s="56" t="s">
-        <v>3</v>
+      <c r="F6" s="54" t="s">
+        <v>1</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="H6" s="34">
+      <c r="H6" s="33">
         <v>0.92230599999999996</v>
       </c>
-      <c r="I6" s="34">
+      <c r="I6" s="33">
         <v>0.90977399999999997</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="33">
         <v>0.90476199999999996</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="33">
         <v>0.90225599999999995</v>
       </c>
-      <c r="L6" s="26">
+      <c r="L6" s="25">
         <v>0.86967399999999995</v>
       </c>
       <c r="M6" s="15"/>
@@ -1167,30 +1179,30 @@
       <c r="R6" s="7"/>
     </row>
     <row r="7" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="56"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="1">
         <v>4</v>
       </c>
       <c r="D7" s="16">
         <v>0.84199999999999997</v>
       </c>
-      <c r="F7" s="56"/>
+      <c r="F7" s="54"/>
       <c r="G7" s="1">
         <v>2</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="33">
         <v>0.95488700000000004</v>
       </c>
-      <c r="I7" s="34">
+      <c r="I7" s="33">
         <v>0.94486199999999998</v>
       </c>
-      <c r="J7" s="34">
+      <c r="J7" s="33">
         <v>0.93984999999999996</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7" s="33">
         <v>0.93734300000000004</v>
       </c>
-      <c r="L7" s="26">
+      <c r="L7" s="25">
         <v>0.90225599999999995</v>
       </c>
       <c r="M7" s="15"/>
@@ -1201,30 +1213,30 @@
       <c r="R7" s="15"/>
     </row>
     <row r="8" spans="2:18" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="57"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="9">
         <v>5</v>
       </c>
       <c r="D8" s="18">
         <v>0.84199999999999997</v>
       </c>
-      <c r="F8" s="56"/>
+      <c r="F8" s="54"/>
       <c r="G8" s="1">
         <v>3</v>
       </c>
-      <c r="H8" s="34">
+      <c r="H8" s="33">
         <v>0.96240599999999998</v>
       </c>
-      <c r="I8" s="34">
+      <c r="I8" s="33">
         <v>0.95238100000000003</v>
       </c>
-      <c r="J8" s="34">
+      <c r="J8" s="33">
         <v>0.94987500000000002</v>
       </c>
-      <c r="K8" s="34">
+      <c r="K8" s="33">
         <v>0.94486199999999998</v>
       </c>
-      <c r="L8" s="26">
+      <c r="L8" s="25">
         <v>0.91228100000000001</v>
       </c>
       <c r="M8" s="15"/>
@@ -1235,67 +1247,67 @@
       <c r="R8" s="15"/>
     </row>
     <row r="9" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="55" t="s">
-        <v>4</v>
+      <c r="B9" s="53" t="s">
+        <v>2</v>
       </c>
       <c r="C9" s="12">
         <v>0.5</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>0.88200000000000001</v>
       </c>
-      <c r="F9" s="56"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="1">
         <v>4</v>
       </c>
-      <c r="H9" s="34">
+      <c r="H9" s="33">
         <v>0.95238100000000003</v>
       </c>
-      <c r="I9" s="34">
+      <c r="I9" s="33">
         <v>0.94736799999999999</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="33">
         <v>0.94736799999999999</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9" s="33">
         <v>0.94486199999999998</v>
       </c>
-      <c r="L9" s="26">
+      <c r="L9" s="25">
         <v>0.91228100000000001</v>
       </c>
       <c r="M9" s="15"/>
     </row>
     <row r="10" spans="2:18" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="56"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="1">
         <v>0.6</v>
       </c>
       <c r="D10" s="16">
         <v>0.90200000000000002</v>
       </c>
-      <c r="F10" s="57"/>
+      <c r="F10" s="55"/>
       <c r="G10" s="9">
         <v>5</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="26">
         <v>0.95488700000000004</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="26">
         <v>0.94987500000000002</v>
       </c>
-      <c r="J10" s="27">
+      <c r="J10" s="26">
         <v>0.94987500000000002</v>
       </c>
-      <c r="K10" s="27">
+      <c r="K10" s="26">
         <v>0.94736799999999999</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="27">
         <v>0.91478700000000002</v>
       </c>
       <c r="M10" s="15"/>
     </row>
     <row r="11" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="56"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="1">
         <v>0.7</v>
       </c>
@@ -1305,7 +1317,7 @@
       <c r="M11" s="15"/>
     </row>
     <row r="12" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="56"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="1">
         <v>0.8</v>
       </c>
@@ -1315,78 +1327,78 @@
       <c r="M12" s="2"/>
     </row>
     <row r="13" spans="2:18" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="57"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="9">
         <v>0.9</v>
       </c>
       <c r="D13" s="18">
         <v>0.91700000000000004</v>
       </c>
-      <c r="F13" s="30"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
+      <c r="F13" s="29"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
     </row>
     <row r="14" spans="2:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="30"/>
+      <c r="B14" s="29"/>
       <c r="D14" s="15"/>
-      <c r="F14" s="30"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
+      <c r="F14" s="29"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
       <c r="M14" s="15"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B15" s="30"/>
+      <c r="B15" s="29"/>
       <c r="D15" s="15"/>
-      <c r="F15" s="30"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
+      <c r="F15" s="29"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33"/>
+      <c r="K15" s="33"/>
+      <c r="L15" s="33"/>
       <c r="M15" s="15"/>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B16" s="30"/>
+      <c r="B16" s="29"/>
       <c r="D16" s="15"/>
-      <c r="F16" s="30"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
+      <c r="F16" s="29"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
       <c r="M16" s="15"/>
     </row>
     <row r="17" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="30"/>
+      <c r="B17" s="29"/>
       <c r="D17" s="15"/>
-      <c r="F17" s="30"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
+      <c r="F17" s="29"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
     </row>
     <row r="18" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="30"/>
+      <c r="B18" s="29"/>
       <c r="D18" s="15"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
@@ -1398,12 +1410,12 @@
       <c r="T19" s="7"/>
     </row>
     <row r="20" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F20" s="37"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
@@ -1415,12 +1427,12 @@
       <c r="T20" s="7"/>
     </row>
     <row r="21" spans="2:20" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="37"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
@@ -1432,12 +1444,12 @@
       <c r="T21" s="7"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="F22" s="37"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
@@ -1449,13 +1461,13 @@
       <c r="T22" s="7"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D23" s="30"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
+      <c r="D23" s="29"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
@@ -1467,9 +1479,9 @@
       <c r="T23" s="7"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D24" s="30"/>
+      <c r="D24" s="29"/>
       <c r="F24" s="15"/>
-      <c r="K24" s="30"/>
+      <c r="K24" s="29"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
@@ -1481,9 +1493,9 @@
       <c r="T24" s="7"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D25" s="30"/>
+      <c r="D25" s="29"/>
       <c r="F25" s="15"/>
-      <c r="K25" s="30"/>
+      <c r="K25" s="29"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
@@ -1495,7 +1507,7 @@
       <c r="T25" s="7"/>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D26" s="30"/>
+      <c r="D26" s="29"/>
       <c r="F26" s="15"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
@@ -1508,7 +1520,7 @@
       <c r="T26" s="7"/>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D27" s="30"/>
+      <c r="D27" s="29"/>
       <c r="F27" s="15"/>
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
@@ -1521,7 +1533,7 @@
       <c r="T27" s="7"/>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D28" s="30"/>
+      <c r="D28" s="29"/>
       <c r="F28" s="15"/>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
@@ -1534,27 +1546,27 @@
       <c r="T28" s="7"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D29" s="30"/>
+      <c r="D29" s="29"/>
       <c r="F29" s="15"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D30" s="30"/>
+      <c r="D30" s="29"/>
       <c r="F30" s="15"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D31" s="30"/>
+      <c r="D31" s="29"/>
       <c r="F31" s="15"/>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="D32" s="30"/>
+      <c r="D32" s="29"/>
       <c r="F32" s="15"/>
     </row>
     <row r="33" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D33" s="30"/>
+      <c r="D33" s="29"/>
       <c r="F33" s="15"/>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D34" s="30"/>
+      <c r="D34" s="29"/>
       <c r="F34" s="15"/>
     </row>
   </sheetData>
@@ -1585,10 +1597,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD0E853E-51FD-9145-8DA3-30D891509AAC}">
-  <dimension ref="B1:P29"/>
+  <dimension ref="B1:P37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -1621,414 +1633,510 @@
       <c r="N1" s="7"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="33"/>
-      <c r="D2" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="73"/>
+      <c r="B2" s="32"/>
+      <c r="D2" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="65"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="42" t="s">
+      <c r="B3" s="32"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="44" t="s">
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="67"/>
+      <c r="F4" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="83">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="75"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="84">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="73"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="32"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="83">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="75"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="68"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="84">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="73"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="68"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="83">
+        <v>0.87</v>
+      </c>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="75"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="68"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="85">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="71"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="74" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="75"/>
-      <c r="F4" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="76">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="77"/>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="67"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="78">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="79"/>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="33"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="80">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="81"/>
-      <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="67"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="78">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="79"/>
-      <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="67"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="80">
-        <v>0.87</v>
-      </c>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="81"/>
-      <c r="N8" s="7"/>
-    </row>
-    <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="67"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="76">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="77"/>
-      <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="22"/>
-      <c r="G10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="38">
+      <c r="F10" s="87" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="88"/>
+      <c r="H10" s="47">
         <v>0.436</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="37">
         <v>0.36599999999999999</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="37">
         <v>0.45400000000000001</v>
       </c>
-      <c r="K10" s="38">
+      <c r="K10" s="37">
         <v>0.79900000000000004</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10" s="38">
         <v>0.81699999999999995</v>
       </c>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="64"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67" t="s">
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="2">
+      <c r="H11" s="48">
         <v>0.54400000000000004</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="82">
         <v>0.43099999999999999</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="82">
         <v>0.58599999999999997</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="82">
         <v>0.77200000000000002</v>
       </c>
-      <c r="L11" s="43">
+      <c r="L11" s="42">
         <v>0.78400000000000003</v>
       </c>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D12" s="64"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
       <c r="G12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="2">
+        <v>14</v>
+      </c>
+      <c r="H12" s="48">
         <v>0.50600000000000001</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="82">
         <v>0.61899999999999999</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="82">
         <v>0.48099999999999998</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="82">
         <v>0.85199999999999998</v>
       </c>
-      <c r="L12" s="43">
+      <c r="L12" s="42">
         <v>0.77700000000000002</v>
       </c>
       <c r="O12" s="21"/>
       <c r="P12" s="21"/>
     </row>
     <row r="13" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="64"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="68"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
       <c r="G13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="40">
+        <v>22</v>
+      </c>
+      <c r="H13" s="51">
         <v>0.47599999999999998</v>
       </c>
-      <c r="I13" s="40">
+      <c r="I13" s="39">
         <v>0.624</v>
       </c>
-      <c r="J13" s="40">
+      <c r="J13" s="39">
         <v>0.41399999999999998</v>
       </c>
-      <c r="K13" s="40">
+      <c r="K13" s="39">
         <v>0.752</v>
       </c>
-      <c r="L13" s="41">
+      <c r="L13" s="40">
         <v>0.52400000000000002</v>
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
     </row>
-    <row r="14" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D14" s="64"/>
-      <c r="E14" s="66" t="s">
-        <v>1</v>
-      </c>
-      <c r="F14" s="46"/>
-      <c r="G14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H14" s="2">
+    <row r="14" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="77"/>
+      <c r="E14" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="87" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="88"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="38"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="48"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="42"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="48"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="82"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="42"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+    </row>
+    <row r="17" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="77"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="51"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="40"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+    </row>
+    <row r="18" spans="4:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="77"/>
+      <c r="E18" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="87" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="88"/>
+      <c r="H18" s="48">
         <v>0.41399999999999998</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I18" s="82">
         <v>0.36099999999999999</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J18" s="82">
         <v>0.52100000000000002</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K18" s="82">
         <v>0.83499999999999996</v>
       </c>
-      <c r="L14" s="43">
+      <c r="L18" s="42">
         <v>0.80200000000000005</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="64"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67" t="s">
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+    </row>
+    <row r="19" spans="4:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="2">
+      <c r="H19" s="48">
         <v>0.38300000000000001</v>
       </c>
-      <c r="I15" s="2">
+      <c r="I19" s="82">
         <v>0.36299999999999999</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J19" s="82">
         <v>0.629</v>
       </c>
-      <c r="K15" s="2">
+      <c r="K19" s="82">
         <v>0.82199999999999995</v>
       </c>
-      <c r="L15" s="43">
+      <c r="L19" s="42">
         <v>0.77700000000000002</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D16" s="64"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="2">
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D20" s="77"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="48">
         <v>0.39100000000000001</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I20" s="82">
         <v>0.42099999999999999</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J20" s="82">
         <v>0.64700000000000002</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K20" s="82">
         <v>0.82699999999999996</v>
       </c>
-      <c r="L16" s="43">
+      <c r="L20" s="42">
         <v>0.77900000000000003</v>
       </c>
-      <c r="N16" s="4"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-    </row>
-    <row r="17" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="65"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="40">
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+    </row>
+    <row r="21" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="77"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="51">
         <v>0.373</v>
       </c>
-      <c r="I17" s="40">
+      <c r="I21" s="39">
         <v>0.42399999999999999</v>
       </c>
-      <c r="J17" s="40">
+      <c r="J21" s="39">
         <v>0.56399999999999995</v>
       </c>
-      <c r="K17" s="40">
+      <c r="K21" s="39">
         <v>0.76200000000000001</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L21" s="40">
         <v>0.81499999999999995</v>
       </c>
-      <c r="N17" s="4"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-    </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="N18" s="4"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-    </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="N19" s="4"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-    </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="N20" s="4"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-    </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-    </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-    </row>
-    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-    </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
-    </row>
-    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+    </row>
+    <row r="22" spans="4:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="77"/>
+      <c r="E22" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="87" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="88"/>
+      <c r="H22" s="48"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="42"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+    </row>
+    <row r="23" spans="4:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="48"/>
+      <c r="I23" s="82"/>
+      <c r="J23" s="82"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="42"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+    </row>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D24" s="77"/>
+      <c r="E24" s="77"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="48"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="42"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+    </row>
+    <row r="25" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="51"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="40"/>
+      <c r="N25" s="4"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
     </row>
     <row r="26" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="N26" s="4"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
     </row>
     <row r="27" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="N27" s="4"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
     </row>
     <row r="28" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="N28" s="4"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
     </row>
@@ -2036,8 +2144,53 @@
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
     </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+    </row>
+    <row r="35" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+    </row>
+    <row r="36" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+    </row>
+    <row r="37" spans="15:16" x14ac:dyDescent="0.25">
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="25">
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D10:D25"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E9"/>
@@ -2050,13 +2203,8 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="H9:L9"/>
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F15:F17"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:L17">
+  <conditionalFormatting sqref="H4:L25">
     <cfRule type="colorScale" priority="153">
       <colorScale>
         <cfvo type="min"/>
@@ -2075,10 +2223,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B03C0B-9DE5-2F4B-9C2D-1DAFD1F29915}">
-  <dimension ref="B1:P27"/>
+  <dimension ref="B1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2111,193 +2259,193 @@
       <c r="N1" s="7"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B2" s="33"/>
-      <c r="D2" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70" t="s">
+      <c r="B2" s="32"/>
+      <c r="D2" s="61" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="65"/>
+      <c r="N2" s="7"/>
+    </row>
+    <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="32"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="7"/>
+    </row>
+    <row r="4" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="67"/>
+      <c r="F4" s="76" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="70">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="71"/>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="68"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="72">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="73"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="32"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="76" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="74">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="75"/>
+      <c r="N6" s="7"/>
+    </row>
+    <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="68"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="72">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="I7" s="72"/>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="73"/>
+      <c r="N7" s="7"/>
+    </row>
+    <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D8" s="68"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="76" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="74">
+        <v>0.87</v>
+      </c>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="75"/>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="68"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" s="70">
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="71"/>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D10" s="76" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="73"/>
-      <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="7"/>
-    </row>
-    <row r="4" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="74" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="75"/>
-      <c r="F4" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="76">
-        <v>0.84199999999999997</v>
-      </c>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="77"/>
-      <c r="N4" s="7"/>
-    </row>
-    <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="67"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="78">
-        <v>0.86699999999999999</v>
-      </c>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="79"/>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="33"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="66" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H6" s="80">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="81"/>
-      <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="67"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="78">
-        <v>0.92700000000000005</v>
-      </c>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="79"/>
-      <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="67"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="66" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="80">
-        <v>0.87</v>
-      </c>
-      <c r="I8" s="80"/>
-      <c r="J8" s="80"/>
-      <c r="K8" s="80"/>
-      <c r="L8" s="81"/>
-      <c r="N8" s="7"/>
-    </row>
-    <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="67"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="76">
-        <v>0.96199999999999997</v>
-      </c>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="77"/>
-      <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="66" t="s">
-        <v>9</v>
-      </c>
       <c r="G10" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="38">
+        <v>8</v>
+      </c>
+      <c r="H10" s="37">
         <v>0.622</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="37">
         <v>0.63900000000000001</v>
       </c>
-      <c r="J10" s="38">
+      <c r="J10" s="37">
         <v>0.77700000000000002</v>
       </c>
-      <c r="K10" s="38">
+      <c r="K10" s="37">
         <v>0.81699999999999995</v>
       </c>
-      <c r="L10" s="39">
+      <c r="L10" s="38">
         <v>0.83699999999999997</v>
       </c>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D11" s="64"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
       <c r="G11" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H11" s="2">
         <v>0.54900000000000004</v>
@@ -2311,7 +2459,7 @@
       <c r="K11" s="2">
         <v>0.86499999999999999</v>
       </c>
-      <c r="L11" s="43">
+      <c r="L11" s="42">
         <v>0.86199999999999999</v>
       </c>
       <c r="N11" s="4"/>
@@ -2319,166 +2467,279 @@
       <c r="P11" s="8"/>
     </row>
     <row r="12" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="64"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="68"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
       <c r="G12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="40">
+        <v>22</v>
+      </c>
+      <c r="H12" s="39">
         <v>0.56599999999999995</v>
       </c>
-      <c r="I12" s="40">
+      <c r="I12" s="39">
         <v>0.63200000000000001</v>
       </c>
-      <c r="J12" s="40">
+      <c r="J12" s="39">
         <v>0.79700000000000004</v>
       </c>
-      <c r="K12" s="40">
+      <c r="K12" s="39">
         <v>0.92700000000000005</v>
       </c>
-      <c r="L12" s="41">
+      <c r="L12" s="40">
         <v>0.95499999999999996</v>
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
     </row>
-    <row r="13" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="64"/>
-      <c r="E13" s="67" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="67" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="D13" s="77"/>
+      <c r="E13" s="77" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="76" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="38"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="82"/>
+      <c r="L14" s="42"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+    </row>
+    <row r="15" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="40"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="D16" s="77"/>
+      <c r="E16" s="77" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="2">
         <v>0.49099999999999999</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I16" s="2">
         <v>0.79200000000000004</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J16" s="2">
         <v>0.76900000000000002</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K16" s="2">
         <v>0.83499999999999996</v>
       </c>
-      <c r="L13" s="43">
+      <c r="L16" s="42">
         <v>0.82</v>
       </c>
-      <c r="N13" s="4"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D14" s="64"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="2">
+      <c r="N16" s="4"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="2">
         <v>0.45600000000000002</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I17" s="2">
         <v>0.47099999999999997</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J17" s="2">
         <v>0.88200000000000001</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K17" s="2">
         <v>0.91</v>
       </c>
-      <c r="L14" s="43">
+      <c r="L17" s="42">
         <v>0.89</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-    </row>
-    <row r="15" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="65"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H15" s="40">
+      <c r="N17" s="4"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+    </row>
+    <row r="18" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="78"/>
+      <c r="G18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="39">
         <v>0.46600000000000003</v>
       </c>
-      <c r="I15" s="40">
+      <c r="I18" s="39">
         <v>0.77900000000000003</v>
       </c>
-      <c r="J15" s="40">
+      <c r="J18" s="39">
         <v>0.80500000000000005</v>
       </c>
-      <c r="K15" s="40">
+      <c r="K18" s="39">
         <v>0.96</v>
       </c>
-      <c r="L15" s="41">
+      <c r="L18" s="40">
         <v>0.88200000000000001</v>
       </c>
-      <c r="N15" s="4"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="N16" s="4"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-    </row>
-    <row r="17" spans="14:16" x14ac:dyDescent="0.2">
-      <c r="N17" s="4"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-    </row>
-    <row r="18" spans="14:16" x14ac:dyDescent="0.2">
       <c r="N18" s="4"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-    </row>
-    <row r="19" spans="14:16" x14ac:dyDescent="0.2">
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="4:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="77"/>
+      <c r="E19" s="68" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="77" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="42"/>
+      <c r="N19" s="4"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D20" s="77"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="42"/>
+      <c r="N20" s="4"/>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="78"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="78"/>
+      <c r="G21" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="40"/>
+      <c r="N21" s="4"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="N22" s="4"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="N23" s="4"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="N24" s="4"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="4:16" x14ac:dyDescent="0.2">
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="4:16" x14ac:dyDescent="0.2">
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="14:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:16" x14ac:dyDescent="0.2">
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="15:16" x14ac:dyDescent="0.2">
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="21">
+    <mergeCell ref="D10:D21"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="E16:E18"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E9"/>
@@ -2491,13 +2752,8 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="H9:L9"/>
-    <mergeCell ref="D10:D15"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:L15">
+  <conditionalFormatting sqref="H4:L21">
     <cfRule type="colorScale" priority="154">
       <colorScale>
         <cfvo type="min"/>
@@ -2518,8 +2774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D718D1-05D9-2146-B7ED-D601D310FD08}">
   <dimension ref="C1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2548,35 +2804,35 @@
   <sheetData>
     <row r="1" spans="3:8" ht="20" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:8" ht="41" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="82"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="47" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="48" t="s">
-        <v>38</v>
+      <c r="C2" s="79"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="46" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C3" s="61" t="s">
-        <v>35</v>
+      <c r="C3" s="59" t="s">
+        <v>33</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="49">
+        <v>11</v>
+      </c>
+      <c r="E3" s="47">
         <v>0.84199999999999997</v>
       </c>
       <c r="F3" s="12">
         <v>0.877</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="37">
         <v>0.92</v>
       </c>
       <c r="H3" s="13">
@@ -2584,11 +2840,11 @@
       </c>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C4" s="61"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="50">
+        <v>12</v>
+      </c>
+      <c r="E4" s="48">
         <v>0.92700000000000005</v>
       </c>
       <c r="F4" s="1">
@@ -2602,13 +2858,13 @@
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="50">
+      <c r="E5" s="48">
         <v>0.87</v>
       </c>
       <c r="F5" s="1">
@@ -2622,11 +2878,11 @@
       </c>
     </row>
     <row r="6" spans="3:8" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="84"/>
+      <c r="C6" s="81"/>
       <c r="D6" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="53">
+        <v>12</v>
+      </c>
+      <c r="E6" s="51">
         <v>0.96199999999999997</v>
       </c>
       <c r="F6" s="9">
@@ -2635,7 +2891,7 @@
       <c r="G6" s="9">
         <v>0.96499999999999997</v>
       </c>
-      <c r="H6" s="54">
+      <c r="H6" s="52">
         <v>0.94199999999999995</v>
       </c>
     </row>

</xml_diff>

<commit_message>
genete more cot tokens
</commit_message>
<xml_diff>
--- a/misc/union_results.xlsx
+++ b/misc/union_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B84EA54-3E99-654B-B785-D54CDE1F8B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398E394C-18BA-9B45-8E03-719B2D0EF833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
@@ -1594,7 +1594,7 @@
   <dimension ref="B1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2082,7 +2082,7 @@
   <dimension ref="B1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated part of cot results; more promising than previous
</commit_message>
<xml_diff>
--- a/misc/union_results.xlsx
+++ b/misc/union_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D784718C-D354-3347-85B5-71DB8A0A7571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D2D925-FF66-504F-8FBD-D7E61EA4F69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="5380" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -581,6 +581,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -605,12 +620,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -629,9 +638,6 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -639,12 +645,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1628,27 +1628,27 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="32"/>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62" t="s">
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="65"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="70"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="32"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
       <c r="H3" s="41" t="s">
         <v>35</v>
       </c>
@@ -1670,124 +1670,124 @@
       <c r="B4" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="69" t="s">
+      <c r="E4" s="72"/>
+      <c r="F4" s="63" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="71">
+      <c r="H4" s="74">
         <v>0.84199999999999997</v>
       </c>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="73"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="76"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="70"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="65"/>
       <c r="G5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="74">
+      <c r="H5" s="77">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="76"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="79"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="32"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="69" t="s">
+      <c r="D6" s="73"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="63" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="71">
+      <c r="H6" s="74">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="73"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="76"/>
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="68"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="70"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="65"/>
       <c r="G7" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="74">
+      <c r="H7" s="77">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="76"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="79"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="68"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="69" t="s">
+      <c r="D8" s="73"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="63" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="71">
+      <c r="H8" s="74">
         <v>0.87</v>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="73"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="76"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="68"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="77"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="64"/>
       <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="78">
+      <c r="H9" s="80">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="80"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="82"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="E10" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="81" t="s">
+      <c r="F10" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="82"/>
+      <c r="G10" s="62"/>
       <c r="H10" s="47">
         <v>0.436</v>
       </c>
@@ -1807,9 +1807,9 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77" t="s">
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1834,9 +1834,9 @@
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
       <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1859,9 +1859,9 @@
       <c r="P12" s="21"/>
     </row>
     <row r="13" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="77"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
       <c r="G13" s="9" t="s">
         <v>22</v>
       </c>
@@ -1884,14 +1884,14 @@
       <c r="P13" s="6"/>
     </row>
     <row r="14" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="77"/>
-      <c r="E14" s="69" t="s">
+      <c r="D14" s="64"/>
+      <c r="E14" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="81" t="s">
+      <c r="F14" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="82"/>
+      <c r="G14" s="62"/>
       <c r="H14" s="48">
         <v>0.41399999999999998</v>
       </c>
@@ -1911,9 +1911,9 @@
       <c r="P14" s="6"/>
     </row>
     <row r="15" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77" t="s">
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1938,9 +1938,9 @@
       <c r="P15" s="6"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
       <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1963,9 +1963,9 @@
       <c r="P16" s="6"/>
     </row>
     <row r="17" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="65"/>
       <c r="G17" s="9" t="s">
         <v>22</v>
       </c>
@@ -2040,13 +2040,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F10:G10"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E9"/>
@@ -2059,6 +2052,13 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="H9:L9"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D10:D17"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F10:G10"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L17">
     <cfRule type="colorScale" priority="157">
@@ -2082,7 +2082,7 @@
   <dimension ref="B1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2116,27 +2116,27 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="32"/>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62" t="s">
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="62"/>
-      <c r="L2" s="65"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="70"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="32"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
       <c r="H3" s="41" t="s">
         <v>35</v>
       </c>
@@ -2158,121 +2158,121 @@
       <c r="B4" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="67"/>
-      <c r="F4" s="69" t="s">
+      <c r="E4" s="72"/>
+      <c r="F4" s="63" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="79">
+      <c r="H4" s="81">
         <v>0.84199999999999997</v>
       </c>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="80"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="82"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="68"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="70"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="65"/>
       <c r="G5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="75">
+      <c r="H5" s="78">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="76"/>
+      <c r="I5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="78"/>
+      <c r="L5" s="79"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="32"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="69" t="s">
+      <c r="D6" s="73"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="63" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="72">
+      <c r="H6" s="75">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I6" s="72"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="73"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="76"/>
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="68"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="70"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="65"/>
       <c r="G7" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="75">
+      <c r="H7" s="78">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="76"/>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="78"/>
+      <c r="L7" s="79"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="68"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="69" t="s">
+      <c r="D8" s="73"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="63" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="72">
+      <c r="H8" s="75">
         <v>0.87</v>
       </c>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="73"/>
+      <c r="I8" s="75"/>
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="76"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="68"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="77"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="64"/>
       <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="79">
+      <c r="H9" s="81">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="80"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="82"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="69" t="s">
+      <c r="D10" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="69" t="s">
+      <c r="E10" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="69" t="s">
+      <c r="F10" s="63" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="12" t="s">
@@ -2297,9 +2297,9 @@
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="64"/>
       <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2323,9 +2323,9 @@
       <c r="P11" s="8"/>
     </row>
     <row r="12" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="77"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
       <c r="G12" s="9" t="s">
         <v>22</v>
       </c>
@@ -2349,11 +2349,11 @@
       <c r="P12" s="8"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D13" s="77"/>
-      <c r="E13" s="69" t="s">
+      <c r="D13" s="64"/>
+      <c r="E13" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="69" t="s">
+      <c r="F13" s="63" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="12" t="s">
@@ -2361,7 +2361,9 @@
       </c>
       <c r="H13" s="37"/>
       <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
+      <c r="J13" s="37">
+        <v>0.81</v>
+      </c>
       <c r="K13" s="37"/>
       <c r="L13" s="38"/>
       <c r="N13" s="4"/>
@@ -2369,15 +2371,17 @@
       <c r="P13" s="8"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="64"/>
+      <c r="F14" s="64"/>
       <c r="G14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2">
+        <v>0.63900000000000001</v>
+      </c>
       <c r="K14" s="2"/>
       <c r="L14" s="42"/>
       <c r="N14" s="4"/>
@@ -2385,15 +2389,17 @@
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="77"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
       <c r="G15" s="9" t="s">
         <v>22</v>
       </c>
       <c r="H15" s="39"/>
       <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
+      <c r="J15" s="39">
+        <v>0.79400000000000004</v>
+      </c>
       <c r="K15" s="39"/>
       <c r="L15" s="40"/>
       <c r="N15" s="4"/>
@@ -2401,11 +2407,11 @@
       <c r="P15" s="8"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D16" s="77"/>
-      <c r="E16" s="69" t="s">
+      <c r="D16" s="64"/>
+      <c r="E16" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="77" t="s">
+      <c r="F16" s="64" t="s">
         <v>7</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -2431,9 +2437,9 @@
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="4:16" x14ac:dyDescent="0.2">
-      <c r="D17" s="77"/>
-      <c r="E17" s="77"/>
-      <c r="F17" s="77"/>
+      <c r="D17" s="64"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="64"/>
       <c r="G17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2457,9 +2463,9 @@
       <c r="P17" s="8"/>
     </row>
     <row r="18" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="77"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
       <c r="G18" s="9" t="s">
         <v>22</v>
       </c>
@@ -2483,11 +2489,11 @@
       <c r="P18" s="8"/>
     </row>
     <row r="19" spans="4:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="77"/>
-      <c r="E19" s="68" t="s">
+      <c r="D19" s="64"/>
+      <c r="E19" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="77" t="s">
+      <c r="F19" s="64" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -2495,7 +2501,9 @@
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="J19" s="2">
+        <v>0.79200000000000004</v>
+      </c>
       <c r="K19" s="2"/>
       <c r="L19" s="42"/>
       <c r="N19" s="4"/>
@@ -2503,15 +2511,17 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.2">
-      <c r="D20" s="77"/>
-      <c r="E20" s="68"/>
-      <c r="F20" s="77"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="64"/>
       <c r="G20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="J20" s="2">
+        <v>0.875</v>
+      </c>
       <c r="K20" s="2"/>
       <c r="L20" s="42"/>
       <c r="N20" s="4"/>
@@ -2519,15 +2529,17 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="70"/>
+      <c r="D21" s="65"/>
       <c r="E21" s="83"/>
-      <c r="F21" s="70"/>
+      <c r="F21" s="65"/>
       <c r="G21" s="9" t="s">
         <v>22</v>
       </c>
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
+      <c r="J21" s="39">
+        <v>0.79700000000000004</v>
+      </c>
       <c r="K21" s="39"/>
       <c r="L21" s="40"/>
       <c r="N21" s="4"/>
@@ -2587,15 +2599,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D10:D21"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="E16:E18"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E9"/>
@@ -2608,6 +2611,15 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="H9:L9"/>
+    <mergeCell ref="D10:D21"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="E16:E18"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L21">
     <cfRule type="colorScale" priority="154">

</xml_diff>

<commit_message>
finished union cot results
</commit_message>
<xml_diff>
--- a/misc/union_results.xlsx
+++ b/misc/union_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binhan/Documents/projects/2024-spatial-data-integration-github/misc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1519D551-5ACA-EB4B-A9A5-10FB57883C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C512A07-0BE7-324E-815C-31FD3E63874F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="4880" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
+    <workbookView xWindow="67200" yWindow="5380" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{2DDB8916-A173-954A-83DE-6DB921889B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="heuristics" sheetId="10" r:id="rId1"/>
@@ -581,63 +581,57 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -645,6 +639,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1628,27 +1628,27 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="32"/>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67" t="s">
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="70"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="65"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="32"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
       <c r="H3" s="41" t="s">
         <v>35</v>
       </c>
@@ -1670,124 +1670,124 @@
       <c r="B4" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="F4" s="63" t="s">
+      <c r="E4" s="67"/>
+      <c r="F4" s="69" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="74">
+      <c r="H4" s="71">
         <v>0.84199999999999997</v>
       </c>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="76"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="73"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="73"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="65"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="77">
+      <c r="H5" s="74">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="79"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="76"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="32"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="63" t="s">
+      <c r="D6" s="68"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="69" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="74">
+      <c r="H6" s="71">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="76"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="73"/>
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="73"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="65"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="77">
+      <c r="H7" s="74">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="79"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="76"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="73"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="63" t="s">
+      <c r="D8" s="68"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="69" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="74">
+      <c r="H8" s="71">
         <v>0.87</v>
       </c>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="76"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="73"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="73"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="64"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="77"/>
       <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="80">
+      <c r="H9" s="78">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="82"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="80"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="61" t="s">
+      <c r="F10" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="62"/>
+      <c r="G10" s="82"/>
       <c r="H10" s="47">
         <v>0.436</v>
       </c>
@@ -1807,9 +1807,9 @@
       <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64" t="s">
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1834,9 +1834,9 @@
       <c r="P11" s="7"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D12" s="64"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
       <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
@@ -1859,9 +1859,9 @@
       <c r="P12" s="21"/>
     </row>
     <row r="13" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="64"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
       <c r="G13" s="9" t="s">
         <v>22</v>
       </c>
@@ -1884,14 +1884,14 @@
       <c r="P13" s="6"/>
     </row>
     <row r="14" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="64"/>
-      <c r="E14" s="63" t="s">
+      <c r="D14" s="77"/>
+      <c r="E14" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="61" t="s">
+      <c r="F14" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="G14" s="62"/>
+      <c r="G14" s="82"/>
       <c r="H14" s="48">
         <v>0.41399999999999998</v>
       </c>
@@ -1911,9 +1911,9 @@
       <c r="P14" s="6"/>
     </row>
     <row r="15" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64" t="s">
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1938,9 +1938,9 @@
       <c r="P15" s="6"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="64"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
       <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1963,9 +1963,9 @@
       <c r="P16" s="6"/>
     </row>
     <row r="17" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
       <c r="G17" s="9" t="s">
         <v>22</v>
       </c>
@@ -2040,6 +2040,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D10:D17"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E9"/>
@@ -2052,13 +2059,6 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="H9:L9"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D10:D17"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F10:G10"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L17">
     <cfRule type="colorScale" priority="157">
@@ -2082,7 +2082,7 @@
   <dimension ref="B1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
@@ -2116,27 +2116,27 @@
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" s="32"/>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67" t="s">
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="70"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="65"/>
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="2:16" ht="41" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="32"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
       <c r="H3" s="41" t="s">
         <v>35</v>
       </c>
@@ -2158,121 +2158,121 @@
       <c r="B4" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="72"/>
-      <c r="F4" s="63" t="s">
+      <c r="E4" s="67"/>
+      <c r="F4" s="69" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="81">
+      <c r="H4" s="79">
         <v>0.84199999999999997</v>
       </c>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="82"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="80"/>
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="73"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="65"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="70"/>
       <c r="G5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="78">
+      <c r="H5" s="75">
         <v>0.86699999999999999</v>
       </c>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="79"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="76"/>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="32"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="63" t="s">
+      <c r="D6" s="68"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="69" t="s">
         <v>14</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="75">
+      <c r="H6" s="72">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="76"/>
+      <c r="I6" s="72"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="73"/>
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="73"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="65"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="70"/>
       <c r="G7" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="78">
+      <c r="H7" s="75">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
-      <c r="K7" s="78"/>
-      <c r="L7" s="79"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="76"/>
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="73"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="63" t="s">
+      <c r="D8" s="68"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="69" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="75">
+      <c r="H8" s="72">
         <v>0.87</v>
       </c>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="76"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="73"/>
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="2:16" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="73"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="64"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="77"/>
       <c r="G9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="81">
+      <c r="H9" s="79">
         <v>0.96199999999999997</v>
       </c>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="82"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="80"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="2:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="69" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="12" t="s">
@@ -2297,9 +2297,9 @@
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="64"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
       <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
@@ -2323,9 +2323,9 @@
       <c r="P11" s="8"/>
     </row>
     <row r="12" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="64"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
       <c r="G12" s="9" t="s">
         <v>22</v>
       </c>
@@ -2349,17 +2349,19 @@
       <c r="P12" s="8"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D13" s="64"/>
-      <c r="E13" s="63" t="s">
+      <c r="D13" s="77"/>
+      <c r="E13" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="63" t="s">
+      <c r="F13" s="69" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="37"/>
+      <c r="H13" s="37">
+        <v>0.55600000000000005</v>
+      </c>
       <c r="I13" s="37">
         <v>0.63900000000000001</v>
       </c>
@@ -2377,13 +2379,15 @@
       <c r="P13" s="8"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
       <c r="G14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2">
+        <v>0.58099999999999996</v>
+      </c>
       <c r="I14" s="2">
         <v>0.627</v>
       </c>
@@ -2401,13 +2405,15 @@
       <c r="P14" s="8"/>
     </row>
     <row r="15" spans="2:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="64"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
       <c r="G15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="39"/>
+      <c r="H15" s="39">
+        <v>0.60899999999999999</v>
+      </c>
       <c r="I15" s="39">
         <v>0.63200000000000001</v>
       </c>
@@ -2425,11 +2431,11 @@
       <c r="P15" s="8"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="D16" s="64"/>
-      <c r="E16" s="63" t="s">
+      <c r="D16" s="77"/>
+      <c r="E16" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="77" t="s">
         <v>7</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -2455,9 +2461,9 @@
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="4:16" x14ac:dyDescent="0.2">
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="64"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
       <c r="G17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2481,9 +2487,9 @@
       <c r="P17" s="8"/>
     </row>
     <row r="18" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="64"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
       <c r="G18" s="9" t="s">
         <v>22</v>
       </c>
@@ -2507,17 +2513,19 @@
       <c r="P18" s="8"/>
     </row>
     <row r="19" spans="4:16" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="64"/>
-      <c r="E19" s="73" t="s">
+      <c r="D19" s="77"/>
+      <c r="E19" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="64" t="s">
+      <c r="F19" s="77" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2">
+        <v>0.58599999999999997</v>
+      </c>
       <c r="I19" s="2">
         <v>0.79700000000000004</v>
       </c>
@@ -2535,13 +2543,15 @@
       <c r="P19" s="2"/>
     </row>
     <row r="20" spans="4:16" x14ac:dyDescent="0.2">
-      <c r="D20" s="64"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="64"/>
+      <c r="D20" s="77"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="77"/>
       <c r="G20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2">
+        <v>0.499</v>
+      </c>
       <c r="I20" s="2">
         <v>0.49399999999999999</v>
       </c>
@@ -2559,13 +2569,15 @@
       <c r="P20" s="2"/>
     </row>
     <row r="21" spans="4:16" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="65"/>
+      <c r="D21" s="70"/>
       <c r="E21" s="83"/>
-      <c r="F21" s="65"/>
+      <c r="F21" s="70"/>
       <c r="G21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H21" s="39"/>
+      <c r="H21" s="39">
+        <v>0.51900000000000002</v>
+      </c>
       <c r="I21" s="39">
         <v>0.75700000000000001</v>
       </c>
@@ -2635,6 +2647,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D10:D21"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="E16:E18"/>
     <mergeCell ref="D2:G3"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D4:E9"/>
@@ -2647,15 +2668,6 @@
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="H8:L8"/>
     <mergeCell ref="H9:L9"/>
-    <mergeCell ref="D10:D21"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="E16:E18"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:L21">
     <cfRule type="colorScale" priority="154">

</xml_diff>